<commit_message>
Still having issues with translations and tilts.
But it's worse now.

But I know where it's wrong. Just look at the new screenshot
</commit_message>
<xml_diff>
--- a/MechanicalTurkStuff/PhrasesToRead.xlsx
+++ b/MechanicalTurkStuff/PhrasesToRead.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11440" yWindow="0" windowWidth="25600" windowHeight="18820" tabRatio="500"/>
+    <workbookView xWindow="13640" yWindow="0" windowWidth="18360" windowHeight="18840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1534,7 +1534,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J106"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
@@ -1601,14 +1600,14 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <f>MAX(0, F2- SUM(G2:H2))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" hidden="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -1659,14 +1658,14 @@
         <v>2</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <f>MAX(0, F4- SUM(G4:H4))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" hidden="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>279</v>
       </c>
@@ -1714,11 +1713,11 @@
         <v>3</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f>MAX(0, F6- SUM(G6:H6))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1887,6 +1886,9 @@
       <c r="F12">
         <v>2</v>
       </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
       <c r="I12">
         <f>MAX(0, F12- SUM(G12:H12))</f>
         <v>2</v>
@@ -1982,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -2037,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>109</v>
       </c>
@@ -2085,14 +2087,14 @@
         <v>2</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <f>MAX(0, F19- SUM(G19:H19))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" hidden="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>117</v>
       </c>
@@ -2147,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>125</v>
       </c>
@@ -2173,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>131</v>
       </c>
@@ -2228,7 +2230,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>135</v>
       </c>
@@ -2254,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>137</v>
       </c>
@@ -2331,11 +2333,11 @@
         <v>2</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28">
         <f>MAX(0, F28- SUM(G28:H28))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2367,7 +2369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>179</v>
       </c>
@@ -2422,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>267</v>
       </c>
@@ -2477,7 +2479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>275</v>
       </c>
@@ -2503,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>281</v>
       </c>
@@ -2551,14 +2553,14 @@
         <v>2</v>
       </c>
       <c r="G36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I36">
         <f>MAX(0, F36- SUM(G36:H36))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" hidden="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>285</v>
       </c>
@@ -2584,7 +2586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>287</v>
       </c>
@@ -2632,14 +2634,14 @@
         <v>2</v>
       </c>
       <c r="G39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I39">
         <f>MAX(0, F39- SUM(G39:H39))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" hidden="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -2687,14 +2689,14 @@
         <v>2</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41">
         <f>MAX(0, F41- SUM(G41:H41))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" hidden="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -2720,7 +2722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -2775,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>65</v>
       </c>
@@ -2881,11 +2883,11 @@
         <v>2</v>
       </c>
       <c r="G48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I48">
         <f>MAX(0, F48- SUM(G48:H48))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2910,14 +2912,14 @@
         <v>2</v>
       </c>
       <c r="G49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49">
         <f>MAX(0, F49- SUM(G49:H49))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" hidden="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>105</v>
       </c>
@@ -3023,11 +3025,11 @@
         <v>2</v>
       </c>
       <c r="G53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I53">
         <f>MAX(0, F53- SUM(G53:H53))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -3168,11 +3170,11 @@
         <v>2</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58">
         <f>MAX(0, F58- SUM(G58:H58))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -3204,7 +3206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>157</v>
       </c>
@@ -3259,7 +3261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1">
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>161</v>
       </c>
@@ -3285,7 +3287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1">
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>163</v>
       </c>
@@ -3340,7 +3342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1">
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>175</v>
       </c>
@@ -3504,11 +3506,11 @@
         <v>2</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70">
         <f>MAX(0, F70- SUM(G70:H70))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -3591,11 +3593,11 @@
         <v>2</v>
       </c>
       <c r="G73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I73">
         <f>MAX(0, F73- SUM(G73:H73))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -3701,11 +3703,11 @@
         <v>3</v>
       </c>
       <c r="G77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I77">
         <f>MAX(0, F77- SUM(G77:H77))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3737,7 +3739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1">
+    <row r="79" spans="1:9">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -3792,7 +3794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" hidden="1">
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
         <v>91</v>
       </c>
@@ -3818,7 +3820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1">
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>93</v>
       </c>
@@ -3866,11 +3868,11 @@
         <v>2</v>
       </c>
       <c r="G83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83">
         <f>MAX(0, F83- SUM(G83:H83))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3895,11 +3897,11 @@
         <v>2</v>
       </c>
       <c r="G84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I84">
         <f>MAX(0, F84- SUM(G84:H84))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -4272,11 +4274,11 @@
         <v>2</v>
       </c>
       <c r="G97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I97">
         <f>MAX(0, F97- SUM(G97:H97))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -4329,6 +4331,9 @@
       <c r="F99">
         <v>2</v>
       </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
       <c r="I99">
         <f>MAX(0, F99- SUM(G99:H99))</f>
         <v>2</v>
@@ -4530,20 +4535,15 @@
         <v>2</v>
       </c>
       <c r="G106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I106">
         <f>MAX(0, F106- SUM(G106:H106))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J106">
-    <filterColumn colId="4">
-      <customFilters>
-        <customFilter operator="notEqual" val="*dour*"/>
-      </customFilters>
-    </filterColumn>
     <sortState ref="A2:J106">
       <sortCondition ref="E1:E106"/>
     </sortState>

</xml_diff>

<commit_message>
a whole bunch of stuff
</commit_message>
<xml_diff>
--- a/MechanicalTurkStuff/PhrasesToRead.xlsx
+++ b/MechanicalTurkStuff/PhrasesToRead.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="0" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1592,7 +1592,7 @@
   <dimension ref="A1:K106"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1644,14 +1644,14 @@
         <v>295</v>
       </c>
       <c r="C2" s="3">
-        <f>LEN(A2)</f>
+        <f t="shared" ref="C2:C33" si="0">LEN(A2)</f>
         <v>17</v>
       </c>
       <c r="D2" s="3">
         <v>51</v>
       </c>
       <c r="E2" t="str">
-        <f>CONCATENATE(B2,".",C2,".",D2,"    ",A2)</f>
+        <f t="shared" ref="E2:E33" si="1">CONCATENATE(B2,".",C2,".",D2,"    ",A2)</f>
         <v xml:space="preserve">A.17.51    a nice cold our  </v>
       </c>
       <c r="F2">
@@ -1664,14 +1664,14 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <f>MAX(0, F2- SUM(G2:H2))</f>
+        <f t="shared" ref="I2:I33" si="2">MAX(0, F2- SUM(G2:H2))</f>
         <v>0</v>
       </c>
       <c r="J2" t="s">
         <v>319</v>
       </c>
       <c r="K2">
-        <f>SUM(G2:H2)</f>
+        <f t="shared" ref="K2:K33" si="3">SUM(G2:H2)</f>
         <v>3</v>
       </c>
     </row>
@@ -1683,14 +1683,14 @@
         <v>295</v>
       </c>
       <c r="C3" s="3">
-        <f>LEN(A3)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="D3" s="3">
         <v>135</v>
       </c>
       <c r="E3" t="str">
-        <f>CONCATENATE(B3,".",C3,".",D3,"    ",A3)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.17.135    an ice cold our  </v>
       </c>
       <c r="F3">
@@ -1700,11 +1700,11 @@
         <v>2</v>
       </c>
       <c r="I3">
-        <f>MAX(0, F3- SUM(G3:H3))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K3">
-        <f>SUM(G3:H3)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -1716,14 +1716,14 @@
         <v>295</v>
       </c>
       <c r="C4" s="3">
-        <f>LEN(A4)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>69</v>
       </c>
       <c r="E4" t="str">
-        <f>CONCATENATE(B4,".",C4,".",D4,"    ",A4)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.17.69    a nye scold our  </v>
       </c>
       <c r="F4">
@@ -1733,11 +1733,11 @@
         <v>2</v>
       </c>
       <c r="I4">
-        <f>MAX(0, F4- SUM(G4:H4))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f>SUM(G4:H4)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -1749,14 +1749,14 @@
         <v>295</v>
       </c>
       <c r="C5" s="3">
-        <f>LEN(A5)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D5" s="3">
         <v>109</v>
       </c>
       <c r="E5" t="str">
-        <f>CONCATENATE(B5,".",C5,".",D5,"    ",A5)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.18.109    ah nye scold our  </v>
       </c>
       <c r="F5">
@@ -1766,11 +1766,11 @@
         <v>2</v>
       </c>
       <c r="I5">
-        <f>MAX(0, F5- SUM(G5:H5))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K5">
-        <f>SUM(G5:H5)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -1782,14 +1782,14 @@
         <v>295</v>
       </c>
       <c r="C6" s="3">
-        <f>LEN(A6)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D6" s="3">
         <v>125</v>
       </c>
       <c r="E6" t="str">
-        <f>CONCATENATE(B6,".",C6,".",D6,"    ",A6)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.18.125    an eye scold our  </v>
       </c>
       <c r="F6">
@@ -1799,11 +1799,11 @@
         <v>2</v>
       </c>
       <c r="I6">
-        <f>MAX(0, F6- SUM(G6:H6))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K6">
-        <f>SUM(G6:H6)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -1815,14 +1815,14 @@
         <v>295</v>
       </c>
       <c r="C7" s="3">
-        <f>LEN(A7)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D7" s="3">
         <v>267</v>
       </c>
       <c r="E7" t="str">
-        <f>CONCATENATE(B7,".",C7,".",D7,"    ",A7)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.18.267    on aye scold our  </v>
       </c>
       <c r="F7">
@@ -1832,11 +1832,11 @@
         <v>2</v>
       </c>
       <c r="I7">
-        <f>MAX(0, F7- SUM(G7:H7))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K7">
-        <f>SUM(G7:H7)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -1848,14 +1848,14 @@
         <v>295</v>
       </c>
       <c r="C8" s="3">
-        <f>LEN(A8)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D8" s="3">
         <v>65</v>
       </c>
       <c r="E8" t="str">
-        <f>CONCATENATE(B8,".",C8,".",D8,"    ",A8)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.18.65    a nigh scold our  </v>
       </c>
       <c r="F8">
@@ -1865,11 +1865,11 @@
         <v>2</v>
       </c>
       <c r="I8">
-        <f>MAX(0, F8- SUM(G8:H8))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K8">
-        <f>SUM(G8:H8)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -1881,14 +1881,14 @@
         <v>295</v>
       </c>
       <c r="C9" s="3">
-        <f>LEN(A9)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D9" s="3">
         <v>71</v>
       </c>
       <c r="E9" t="str">
-        <f>CONCATENATE(B9,".",C9,".",D9,"    ",A9)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.18.71    a nye skol dower  </v>
       </c>
       <c r="F9">
@@ -1898,11 +1898,11 @@
         <v>2</v>
       </c>
       <c r="I9">
-        <f>MAX(0, F9- SUM(G9:H9))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K9">
-        <f>SUM(G9:H9)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -1914,14 +1914,14 @@
         <v>295</v>
       </c>
       <c r="C10" s="3">
-        <f>LEN(A10)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="D10" s="3">
         <v>119</v>
       </c>
       <c r="E10" t="str">
-        <f>CONCATENATE(B10,".",C10,".",D10,"    ",A10)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.19.119    an aye skol dower  </v>
       </c>
       <c r="F10">
@@ -1931,11 +1931,11 @@
         <v>2</v>
       </c>
       <c r="I10">
-        <f>MAX(0, F10- SUM(G10:H10))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K10">
-        <f>SUM(G10:H10)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -1947,14 +1947,14 @@
         <v>295</v>
       </c>
       <c r="C11" s="3">
-        <f>LEN(A11)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="D11" s="3">
         <v>127</v>
       </c>
       <c r="E11" t="str">
-        <f>CONCATENATE(B11,".",C11,".",D11,"    ",A11)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.19.127    an eye skol dower  </v>
       </c>
       <c r="F11">
@@ -1964,11 +1964,11 @@
         <v>2</v>
       </c>
       <c r="I11">
-        <f>MAX(0, F11- SUM(G11:H11))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K11">
-        <f>SUM(G11:H11)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -1980,14 +1980,14 @@
         <v>295</v>
       </c>
       <c r="C12" s="3">
-        <f>LEN(A12)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="D12" s="3">
         <v>133</v>
       </c>
       <c r="E12" t="str">
-        <f>CONCATENATE(B12,".",C12,".",D12,"    ",A12)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.19.133    an ice coal dower  </v>
       </c>
       <c r="F12">
@@ -1997,11 +1997,11 @@
         <v>2</v>
       </c>
       <c r="I12">
-        <f>MAX(0, F12- SUM(G12:H12))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K12">
-        <f>SUM(G12:H12)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -2013,14 +2013,14 @@
         <v>295</v>
       </c>
       <c r="C13" s="3">
-        <f>LEN(A13)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="D13" s="3">
         <v>159</v>
       </c>
       <c r="E13" t="str">
-        <f>CONCATENATE(B13,".",C13,".",D13,"    ",A13)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.20.159    eh nice coal dower  </v>
       </c>
       <c r="F13">
@@ -2030,11 +2030,11 @@
         <v>2</v>
       </c>
       <c r="I13">
-        <f>MAX(0, F13- SUM(G13:H13))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K13">
-        <f>SUM(G13:H13)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -2046,14 +2046,14 @@
         <v>295</v>
       </c>
       <c r="C14" s="3">
-        <f>LEN(A14)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="D14" s="3">
         <v>89</v>
       </c>
       <c r="E14" t="str">
-        <f>CONCATENATE(B14,".",C14,".",D14,"    ",A14)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.20.89    ah nice coal dower  </v>
       </c>
       <c r="F14">
@@ -2063,11 +2063,11 @@
         <v>2</v>
       </c>
       <c r="I14">
-        <f>MAX(0, F14- SUM(G14:H14))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K14">
-        <f>SUM(G14:H14)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -2079,14 +2079,14 @@
         <v>296</v>
       </c>
       <c r="C15" s="3">
-        <f>LEN(A15)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="D15" s="3">
         <v>19</v>
       </c>
       <c r="E15" t="str">
-        <f>CONCATENATE(B15,".",C15,".",D15,"    ",A15)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">B.15.19    fourth wry to  </v>
       </c>
       <c r="F15">
@@ -2096,11 +2096,11 @@
         <v>2</v>
       </c>
       <c r="I15">
-        <f>MAX(0, F15- SUM(G15:H15))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K15">
-        <f>SUM(G15:H15)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -2112,14 +2112,14 @@
         <v>296</v>
       </c>
       <c r="C16" s="3">
-        <f>LEN(A16)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D16" s="3">
         <v>20</v>
       </c>
       <c r="E16" t="str">
-        <f>CONCATENATE(B16,".",C16,".",D16,"    ",A16)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">B.16.20    fourth wry too  </v>
       </c>
       <c r="F16">
@@ -2129,11 +2129,11 @@
         <v>2</v>
       </c>
       <c r="I16">
-        <f>MAX(0, F16- SUM(G16:H16))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K16">
-        <f>SUM(G16:H16)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -2145,14 +2145,14 @@
         <v>296</v>
       </c>
       <c r="C17" s="3">
-        <f>LEN(A17)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="D17" s="3">
         <v>1</v>
       </c>
       <c r="E17" t="str">
-        <f>CONCATENATE(B17,".",C17,".",D17,"    ",A17)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">B.17.1    forth right ooh  </v>
       </c>
       <c r="F17">
@@ -2162,11 +2162,11 @@
         <v>2</v>
       </c>
       <c r="I17">
-        <f>MAX(0, F17- SUM(G17:H17))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K17">
-        <f>SUM(G17:H17)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -2178,14 +2178,14 @@
         <v>296</v>
       </c>
       <c r="C18" s="3">
-        <f>LEN(A18)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="D18" s="3">
         <v>13</v>
       </c>
       <c r="E18" t="str">
-        <f>CONCATENATE(B18,".",C18,".",D18,"    ",A18)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">B.17.13    fourth rite ooh  </v>
       </c>
       <c r="F18">
@@ -2195,11 +2195,11 @@
         <v>2</v>
       </c>
       <c r="I18">
-        <f>MAX(0, F18- SUM(G18:H18))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K18">
-        <f>SUM(G18:H18)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -2211,14 +2211,14 @@
         <v>296</v>
       </c>
       <c r="C19" s="3">
-        <f>LEN(A19)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D19" s="3">
         <v>6</v>
       </c>
       <c r="E19" t="str">
-        <f>CONCATENATE(B19,".",C19,".",D19,"    ",A19)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">B.18.6    forth wright ooh  </v>
       </c>
       <c r="F19">
@@ -2228,11 +2228,11 @@
         <v>2</v>
       </c>
       <c r="I19">
-        <f>MAX(0, F19- SUM(G19:H19))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K19">
-        <f>SUM(G19:H19)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -2244,14 +2244,14 @@
         <v>295</v>
       </c>
       <c r="C20" s="3">
-        <f>LEN(A20)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D20" s="3">
         <v>279</v>
       </c>
       <c r="E20" t="str">
-        <f>CONCATENATE(B20,".",C20,".",D20,"    ",A20)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.16.279    on i scold our  </v>
       </c>
       <c r="F20">
@@ -2261,11 +2261,11 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <f>MAX(0, F20- SUM(G20:H20))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K20">
-        <f>SUM(G20:H20)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2277,14 +2277,14 @@
         <v>295</v>
       </c>
       <c r="C21" s="3">
-        <f>LEN(A21)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="D21" s="3">
         <v>128</v>
       </c>
       <c r="E21" t="str">
-        <f>CONCATENATE(B21,".",C21,".",D21,"    ",A21)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.17.128    an i scold hour  </v>
       </c>
       <c r="F21">
@@ -2294,11 +2294,11 @@
         <v>1</v>
       </c>
       <c r="I21">
-        <f>MAX(0, F21- SUM(G21:H21))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K21">
-        <f>SUM(G21:H21)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2310,14 +2310,14 @@
         <v>295</v>
       </c>
       <c r="C22" s="3">
-        <f>LEN(A22)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="D22" s="3">
         <v>131</v>
       </c>
       <c r="E22" t="str">
-        <f>CONCATENATE(B22,".",C22,".",D22,"    ",A22)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.17.131    an i skol dower  </v>
       </c>
       <c r="F22">
@@ -2327,11 +2327,11 @@
         <v>1</v>
       </c>
       <c r="I22">
-        <f>MAX(0, F22- SUM(G22:H22))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K22">
-        <f>SUM(G22:H22)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2343,14 +2343,14 @@
         <v>295</v>
       </c>
       <c r="C23" s="3">
-        <f>LEN(A23)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="D23" s="3">
         <v>141</v>
       </c>
       <c r="E23" t="str">
-        <f>CONCATENATE(B23,".",C23,".",D23,"    ",A23)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.17.141    an ice-cold our  </v>
       </c>
       <c r="F23">
@@ -2360,11 +2360,11 @@
         <v>1</v>
       </c>
       <c r="I23">
-        <f>MAX(0, F23- SUM(G23:H23))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K23">
-        <f>SUM(G23:H23)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2376,14 +2376,14 @@
         <v>295</v>
       </c>
       <c r="C24" s="3">
-        <f>LEN(A24)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="D24" s="3">
         <v>278</v>
       </c>
       <c r="E24" t="str">
-        <f>CONCATENATE(B24,".",C24,".",D24,"    ",A24)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.17.278    on i scold hour  </v>
       </c>
       <c r="F24">
@@ -2393,11 +2393,11 @@
         <v>1</v>
       </c>
       <c r="I24">
-        <f>MAX(0, F24- SUM(G24:H24))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K24">
-        <f>SUM(G24:H24)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2409,14 +2409,14 @@
         <v>295</v>
       </c>
       <c r="C25" s="3">
-        <f>LEN(A25)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="D25" s="3">
         <v>281</v>
       </c>
       <c r="E25" t="str">
-        <f>CONCATENATE(B25,".",C25,".",D25,"    ",A25)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.17.281    on i skol dower  </v>
       </c>
       <c r="F25">
@@ -2426,11 +2426,11 @@
         <v>1</v>
       </c>
       <c r="I25">
-        <f>MAX(0, F25- SUM(G25:H25))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K25">
-        <f>SUM(G25:H25)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2442,14 +2442,14 @@
         <v>295</v>
       </c>
       <c r="C26" s="3">
-        <f>LEN(A26)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D26" s="3">
         <v>117</v>
       </c>
       <c r="E26" t="str">
-        <f>CONCATENATE(B26,".",C26,".",D26,"    ",A26)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.18.117    an aye scold our  </v>
       </c>
       <c r="F26">
@@ -2459,11 +2459,11 @@
         <v>1</v>
       </c>
       <c r="I26">
-        <f>MAX(0, F26- SUM(G26:H26))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K26">
-        <f>SUM(G26:H26)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2475,14 +2475,14 @@
         <v>295</v>
       </c>
       <c r="C27" s="3">
-        <f>LEN(A27)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D27" s="3">
         <v>134</v>
       </c>
       <c r="E27" t="str">
-        <f>CONCATENATE(B27,".",C27,".",D27,"    ",A27)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.18.134    an ice cold hour  </v>
       </c>
       <c r="F27">
@@ -2492,11 +2492,11 @@
         <v>1</v>
       </c>
       <c r="I27">
-        <f>MAX(0, F27- SUM(G27:H27))</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K27">
-        <f>SUM(G27:H27)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2508,14 +2508,14 @@
         <v>295</v>
       </c>
       <c r="C28" s="3">
-        <f>LEN(A28)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D28" s="3">
         <v>140</v>
       </c>
       <c r="E28" t="str">
-        <f>CONCATENATE(B28,".",C28,".",D28,"    ",A28)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.18.140    an ice-cold hour  </v>
       </c>
       <c r="F28">
@@ -2525,11 +2525,11 @@
         <v>1</v>
       </c>
       <c r="I28">
-        <f>MAX(0, F28- SUM(G28:H28))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K28">
-        <f>SUM(G28:H28)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2541,14 +2541,14 @@
         <v>295</v>
       </c>
       <c r="C29" s="3">
-        <f>LEN(A29)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D29" s="3">
         <v>179</v>
       </c>
       <c r="E29" t="str">
-        <f>CONCATENATE(B29,".",C29,".",D29,"    ",A29)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.18.179    eh nye scold our  </v>
       </c>
       <c r="F29">
@@ -2558,11 +2558,11 @@
         <v>1</v>
       </c>
       <c r="I29">
-        <f>MAX(0, F29- SUM(G29:H29))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K29">
-        <f>SUM(G29:H29)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2574,14 +2574,14 @@
         <v>295</v>
       </c>
       <c r="C30" s="3">
-        <f>LEN(A30)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D30" s="3">
         <v>275</v>
       </c>
       <c r="E30" t="str">
-        <f>CONCATENATE(B30,".",C30,".",D30,"    ",A30)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.18.275    on eye scold our  </v>
       </c>
       <c r="F30">
@@ -2591,11 +2591,11 @@
         <v>1</v>
       </c>
       <c r="I30">
-        <f>MAX(0, F30- SUM(G30:H30))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K30">
-        <f>SUM(G30:H30)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2607,14 +2607,14 @@
         <v>295</v>
       </c>
       <c r="C31" s="3">
-        <f>LEN(A31)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D31" s="3">
         <v>284</v>
       </c>
       <c r="E31" t="str">
-        <f>CONCATENATE(B31,".",C31,".",D31,"    ",A31)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.18.284    on ice cold hour  </v>
       </c>
       <c r="F31">
@@ -2624,11 +2624,11 @@
         <v>1</v>
       </c>
       <c r="I31">
-        <f>MAX(0, F31- SUM(G31:H31))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K31">
-        <f>SUM(G31:H31)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2640,14 +2640,14 @@
         <v>295</v>
       </c>
       <c r="C32" s="3">
-        <f>LEN(A32)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D32" s="3">
         <v>290</v>
       </c>
       <c r="E32" t="str">
-        <f>CONCATENATE(B32,".",C32,".",D32,"    ",A32)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.18.290    on ice-cold hour  </v>
       </c>
       <c r="F32">
@@ -2657,11 +2657,11 @@
         <v>1</v>
       </c>
       <c r="I32">
-        <f>MAX(0, F32- SUM(G32:H32))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K32">
-        <f>SUM(G32:H32)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2673,14 +2673,14 @@
         <v>295</v>
       </c>
       <c r="C33" s="3">
-        <f>LEN(A33)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D33" s="3">
         <v>68</v>
       </c>
       <c r="E33" t="str">
-        <f>CONCATENATE(B33,".",C33,".",D33,"    ",A33)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">A.18.68    a nye scold hour  </v>
       </c>
       <c r="F33">
@@ -2690,11 +2690,11 @@
         <v>1</v>
       </c>
       <c r="I33">
-        <f>MAX(0, F33- SUM(G33:H33))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K33">
-        <f>SUM(G33:H33)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2706,14 +2706,14 @@
         <v>295</v>
       </c>
       <c r="C34" s="3">
-        <f>LEN(A34)</f>
+        <f t="shared" ref="C34:C65" si="4">LEN(A34)</f>
         <v>18</v>
       </c>
       <c r="D34" s="3">
         <v>91</v>
       </c>
       <c r="E34" t="str">
-        <f>CONCATENATE(B34,".",C34,".",D34,"    ",A34)</f>
+        <f t="shared" ref="E34:E65" si="5">CONCATENATE(B34,".",C34,".",D34,"    ",A34)</f>
         <v xml:space="preserve">A.18.91    ah nice cold our  </v>
       </c>
       <c r="F34">
@@ -2723,11 +2723,11 @@
         <v>1</v>
       </c>
       <c r="I34">
-        <f>MAX(0, F34- SUM(G34:H34))</f>
+        <f t="shared" ref="I34:I65" si="6">MAX(0, F34- SUM(G34:H34))</f>
         <v>1</v>
       </c>
       <c r="K34">
-        <f>SUM(G34:H34)</f>
+        <f t="shared" ref="K34:K65" si="7">SUM(G34:H34)</f>
         <v>1</v>
       </c>
     </row>
@@ -2739,14 +2739,14 @@
         <v>295</v>
       </c>
       <c r="C35" s="3">
-        <f>LEN(A35)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D35" s="3">
         <v>105</v>
       </c>
       <c r="E35" t="str">
-        <f>CONCATENATE(B35,".",C35,".",D35,"    ",A35)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.105    ah nigh scold our  </v>
       </c>
       <c r="F35">
@@ -2756,11 +2756,11 @@
         <v>1</v>
       </c>
       <c r="I35">
-        <f>MAX(0, F35- SUM(G35:H35))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K35">
-        <f>SUM(G35:H35)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -2772,14 +2772,14 @@
         <v>295</v>
       </c>
       <c r="C36" s="3">
-        <f>LEN(A36)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D36" s="3">
         <v>108</v>
       </c>
       <c r="E36" t="str">
-        <f>CONCATENATE(B36,".",C36,".",D36,"    ",A36)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.108    ah nye scold hour  </v>
       </c>
       <c r="F36">
@@ -2789,11 +2789,11 @@
         <v>1</v>
       </c>
       <c r="I36">
-        <f>MAX(0, F36- SUM(G36:H36))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K36">
-        <f>SUM(G36:H36)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -2805,14 +2805,14 @@
         <v>295</v>
       </c>
       <c r="C37" s="3">
-        <f>LEN(A37)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D37" s="3">
         <v>111</v>
       </c>
       <c r="E37" t="str">
-        <f>CONCATENATE(B37,".",C37,".",D37,"    ",A37)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.111    ah nye skol dower  </v>
       </c>
       <c r="F37">
@@ -2822,11 +2822,11 @@
         <v>1</v>
       </c>
       <c r="I37">
-        <f>MAX(0, F37- SUM(G37:H37))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K37">
-        <f>SUM(G37:H37)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -2838,14 +2838,14 @@
         <v>295</v>
       </c>
       <c r="C38" s="3">
-        <f>LEN(A38)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D38" s="3">
         <v>116</v>
       </c>
       <c r="E38" t="str">
-        <f>CONCATENATE(B38,".",C38,".",D38,"    ",A38)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.116    an aye scold hour  </v>
       </c>
       <c r="F38">
@@ -2855,11 +2855,11 @@
         <v>1</v>
       </c>
       <c r="I38">
-        <f>MAX(0, F38- SUM(G38:H38))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K38">
-        <f>SUM(G38:H38)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -2871,14 +2871,14 @@
         <v>295</v>
       </c>
       <c r="C39" s="3">
-        <f>LEN(A39)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D39" s="3">
         <v>139</v>
       </c>
       <c r="E39" t="str">
-        <f>CONCATENATE(B39,".",C39,".",D39,"    ",A39)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.139    an ice kohl dower  </v>
       </c>
       <c r="F39">
@@ -2888,11 +2888,11 @@
         <v>1</v>
       </c>
       <c r="I39">
-        <f>MAX(0, F39- SUM(G39:H39))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K39">
-        <f>SUM(G39:H39)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -2904,14 +2904,14 @@
         <v>295</v>
       </c>
       <c r="C40" s="3">
-        <f>LEN(A40)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D40" s="3">
         <v>160</v>
       </c>
       <c r="E40" t="str">
-        <f>CONCATENATE(B40,".",C40,".",D40,"    ",A40)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.160    eh nice cold hour  </v>
       </c>
       <c r="F40">
@@ -2921,11 +2921,11 @@
         <v>1</v>
       </c>
       <c r="I40">
-        <f>MAX(0, F40- SUM(G40:H40))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K40">
-        <f>SUM(G40:H40)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -2937,14 +2937,14 @@
         <v>295</v>
       </c>
       <c r="C41" s="3">
-        <f>LEN(A41)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D41" s="3">
         <v>175</v>
       </c>
       <c r="E41" t="str">
-        <f>CONCATENATE(B41,".",C41,".",D41,"    ",A41)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.175    eh nigh scold our  </v>
       </c>
       <c r="F41">
@@ -2954,11 +2954,11 @@
         <v>1</v>
       </c>
       <c r="I41">
-        <f>MAX(0, F41- SUM(G41:H41))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K41">
-        <f>SUM(G41:H41)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -2970,14 +2970,14 @@
         <v>295</v>
       </c>
       <c r="C42" s="3">
-        <f>LEN(A42)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D42" s="3">
         <v>181</v>
       </c>
       <c r="E42" t="str">
-        <f>CONCATENATE(B42,".",C42,".",D42,"    ",A42)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.181    eh nye skol dower  </v>
       </c>
       <c r="F42">
@@ -2987,11 +2987,11 @@
         <v>1</v>
       </c>
       <c r="I42">
-        <f>MAX(0, F42- SUM(G42:H42))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K42">
-        <f>SUM(G42:H42)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3003,14 +3003,14 @@
         <v>295</v>
       </c>
       <c r="C43" s="3">
-        <f>LEN(A43)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D43" s="3">
         <v>269</v>
       </c>
       <c r="E43" t="str">
-        <f>CONCATENATE(B43,".",C43,".",D43,"    ",A43)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.269    on aye skol dower  </v>
       </c>
       <c r="F43">
@@ -3020,11 +3020,11 @@
         <v>1</v>
       </c>
       <c r="I43">
-        <f>MAX(0, F43- SUM(G43:H43))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K43">
-        <f>SUM(G43:H43)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3036,14 +3036,14 @@
         <v>295</v>
       </c>
       <c r="C44" s="3">
-        <f>LEN(A44)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D44" s="3">
         <v>274</v>
       </c>
       <c r="E44" t="str">
-        <f>CONCATENATE(B44,".",C44,".",D44,"    ",A44)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.274    on eye scold hour  </v>
       </c>
       <c r="F44">
@@ -3053,11 +3053,11 @@
         <v>1</v>
       </c>
       <c r="I44">
-        <f>MAX(0, F44- SUM(G44:H44))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K44">
-        <f>SUM(G44:H44)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3069,14 +3069,14 @@
         <v>295</v>
       </c>
       <c r="C45" s="3">
-        <f>LEN(A45)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D45" s="3">
         <v>283</v>
       </c>
       <c r="E45" t="str">
-        <f>CONCATENATE(B45,".",C45,".",D45,"    ",A45)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.283    on ice coal dower  </v>
       </c>
       <c r="F45">
@@ -3086,11 +3086,11 @@
         <v>1</v>
       </c>
       <c r="I45">
-        <f>MAX(0, F45- SUM(G45:H45))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K45">
-        <f>SUM(G45:H45)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3102,14 +3102,14 @@
         <v>295</v>
       </c>
       <c r="C46" s="3">
-        <f>LEN(A46)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D46" s="3">
         <v>289</v>
       </c>
       <c r="E46" t="str">
-        <f>CONCATENATE(B46,".",C46,".",D46,"    ",A46)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.289    on ice kohl dower  </v>
       </c>
       <c r="F46">
@@ -3119,11 +3119,11 @@
         <v>1</v>
       </c>
       <c r="I46">
-        <f>MAX(0, F46- SUM(G46:H46))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K46">
-        <f>SUM(G46:H46)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3135,14 +3135,14 @@
         <v>295</v>
       </c>
       <c r="C47" s="3">
-        <f>LEN(A47)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D47" s="3">
         <v>49</v>
       </c>
       <c r="E47" t="str">
-        <f>CONCATENATE(B47,".",C47,".",D47,"    ",A47)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.49    a nice coal dower  </v>
       </c>
       <c r="F47">
@@ -3152,11 +3152,11 @@
         <v>1</v>
       </c>
       <c r="I47">
-        <f>MAX(0, F47- SUM(G47:H47))</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K47">
-        <f>SUM(G47:H47)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3168,14 +3168,14 @@
         <v>295</v>
       </c>
       <c r="C48" s="3">
-        <f>LEN(A48)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D48" s="3">
         <v>64</v>
       </c>
       <c r="E48" t="str">
-        <f>CONCATENATE(B48,".",C48,".",D48,"    ",A48)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.64    a nigh scold hour  </v>
       </c>
       <c r="F48">
@@ -3185,11 +3185,11 @@
         <v>1</v>
       </c>
       <c r="I48">
-        <f>MAX(0, F48- SUM(G48:H48))</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K48">
-        <f>SUM(G48:H48)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3201,14 +3201,14 @@
         <v>295</v>
       </c>
       <c r="C49" s="3">
-        <f>LEN(A49)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D49" s="3">
         <v>90</v>
       </c>
       <c r="E49" t="str">
-        <f>CONCATENATE(B49,".",C49,".",D49,"    ",A49)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.19.90    ah nice cold hour  </v>
       </c>
       <c r="F49">
@@ -3218,11 +3218,11 @@
         <v>1</v>
       </c>
       <c r="I49">
-        <f>MAX(0, F49- SUM(G49:H49))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K49">
-        <f>SUM(G49:H49)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3234,14 +3234,14 @@
         <v>295</v>
       </c>
       <c r="C50" s="3">
-        <f>LEN(A50)</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="D50" s="3">
         <v>163</v>
       </c>
       <c r="E50" t="str">
-        <f>CONCATENATE(B50,".",C50,".",D50,"    ",A50)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.20.163    eh nice cole dower  </v>
       </c>
       <c r="F50">
@@ -3251,11 +3251,11 @@
         <v>1</v>
       </c>
       <c r="I50">
-        <f>MAX(0, F50- SUM(G50:H50))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K50">
-        <f>SUM(G50:H50)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3267,14 +3267,14 @@
         <v>295</v>
       </c>
       <c r="C51" s="3">
-        <f>LEN(A51)</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="D51" s="3">
         <v>174</v>
       </c>
       <c r="E51" t="str">
-        <f>CONCATENATE(B51,".",C51,".",D51,"    ",A51)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.20.174    eh nigh scold hour  </v>
       </c>
       <c r="F51">
@@ -3284,11 +3284,11 @@
         <v>1</v>
       </c>
       <c r="I51">
-        <f>MAX(0, F51- SUM(G51:H51))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K51">
-        <f>SUM(G51:H51)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3300,14 +3300,14 @@
         <v>295</v>
       </c>
       <c r="C52" s="3">
-        <f>LEN(A52)</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="D52" s="3">
         <v>177</v>
       </c>
       <c r="E52" t="str">
-        <f>CONCATENATE(B52,".",C52,".",D52,"    ",A52)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.20.177    eh nigh skol dower  </v>
       </c>
       <c r="F52">
@@ -3317,11 +3317,11 @@
         <v>1</v>
       </c>
       <c r="I52">
-        <f>MAX(0, F52- SUM(G52:H52))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K52">
-        <f>SUM(G52:H52)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3333,14 +3333,14 @@
         <v>295</v>
       </c>
       <c r="C53" s="3">
-        <f>LEN(A53)</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="D53" s="3">
         <v>93</v>
       </c>
       <c r="E53" t="str">
-        <f>CONCATENATE(B53,".",C53,".",D53,"    ",A53)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.20.93    ah nice cole dower  </v>
       </c>
       <c r="F53">
@@ -3350,11 +3350,11 @@
         <v>1</v>
       </c>
       <c r="I53">
-        <f>MAX(0, F53- SUM(G53:H53))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K53">
-        <f>SUM(G53:H53)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3366,14 +3366,14 @@
         <v>295</v>
       </c>
       <c r="C54" s="3">
-        <f>LEN(A54)</f>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="D54" s="3">
         <v>95</v>
       </c>
       <c r="E54" t="str">
-        <f>CONCATENATE(B54,".",C54,".",D54,"    ",A54)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.20.95    ah nice kohl dower  </v>
       </c>
       <c r="F54">
@@ -3383,11 +3383,11 @@
         <v>1</v>
       </c>
       <c r="I54">
-        <f>MAX(0, F54- SUM(G54:H54))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K54">
-        <f>SUM(G54:H54)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3399,14 +3399,14 @@
         <v>296</v>
       </c>
       <c r="C55" s="3">
-        <f>LEN(A55)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="D55" s="3">
         <v>10</v>
       </c>
       <c r="E55" t="str">
-        <f>CONCATENATE(B55,".",C55,".",D55,"    ",A55)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">B.15.10    forth wry two  </v>
       </c>
       <c r="F55">
@@ -3416,11 +3416,11 @@
         <v>1</v>
       </c>
       <c r="I55">
-        <f>MAX(0, F55- SUM(G55:H55))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K55">
-        <f>SUM(G55:H55)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3432,14 +3432,14 @@
         <v>296</v>
       </c>
       <c r="C56" s="3">
-        <f>LEN(A56)</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="D56" s="3">
         <v>5</v>
       </c>
       <c r="E56" t="str">
-        <f>CONCATENATE(B56,".",C56,".",D56,"    ",A56)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">B.15.5    forth rye two  </v>
       </c>
       <c r="F56">
@@ -3449,11 +3449,11 @@
         <v>1</v>
       </c>
       <c r="I56">
-        <f>MAX(0, F56- SUM(G56:H56))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K56">
-        <f>SUM(G56:H56)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3465,14 +3465,14 @@
         <v>296</v>
       </c>
       <c r="C57" s="3">
-        <f>LEN(A57)</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="D57" s="3">
         <v>7</v>
       </c>
       <c r="E57" t="str">
-        <f>CONCATENATE(B57,".",C57,".",D57,"    ",A57)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">B.17.7    forth write ooh  </v>
       </c>
       <c r="F57">
@@ -3482,11 +3482,11 @@
         <v>1</v>
       </c>
       <c r="I57">
-        <f>MAX(0, F57- SUM(G57:H57))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K57">
-        <f>SUM(G57:H57)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3498,14 +3498,14 @@
         <v>296</v>
       </c>
       <c r="C58" s="3">
-        <f>LEN(A58)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="D58" s="3">
         <v>12</v>
       </c>
       <c r="E58" t="str">
-        <f>CONCATENATE(B58,".",C58,".",D58,"    ",A58)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">B.18.12    fourth right ooh  </v>
       </c>
       <c r="F58">
@@ -3515,11 +3515,11 @@
         <v>1</v>
       </c>
       <c r="I58">
-        <f>MAX(0, F58- SUM(G58:H58))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K58">
-        <f>SUM(G58:H58)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3531,14 +3531,14 @@
         <v>296</v>
       </c>
       <c r="C59" s="3">
-        <f>LEN(A59)</f>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="D59" s="3">
         <v>17</v>
       </c>
       <c r="E59" t="str">
-        <f>CONCATENATE(B59,".",C59,".",D59,"    ",A59)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">B.19.17    fourth wright ooh  </v>
       </c>
       <c r="F59">
@@ -3548,11 +3548,11 @@
         <v>1</v>
       </c>
       <c r="I59">
-        <f>MAX(0, F59- SUM(G59:H59))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K59">
-        <f>SUM(G59:H59)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3564,14 +3564,14 @@
         <v>295</v>
       </c>
       <c r="C60" s="3">
-        <f>LEN(A60)</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="D60" s="3">
         <v>129</v>
       </c>
       <c r="E60" t="str">
-        <f>CONCATENATE(B60,".",C60,".",D60,"    ",A60)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.16.129    an i scold our  </v>
       </c>
       <c r="F60">
@@ -3581,11 +3581,11 @@
         <v>0</v>
       </c>
       <c r="I60">
-        <f>MAX(0, F60- SUM(G60:H60))</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K60">
-        <f>SUM(G60:H60)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3597,14 +3597,14 @@
         <v>295</v>
       </c>
       <c r="C61" s="3">
-        <f>LEN(A61)</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="D61" s="3">
         <v>130</v>
       </c>
       <c r="E61" t="str">
-        <f>CONCATENATE(B61,".",C61,".",D61,"    ",A61)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.16.130    an i skol dour  </v>
       </c>
       <c r="F61">
@@ -3614,11 +3614,11 @@
         <v>0</v>
       </c>
       <c r="I61">
-        <f>MAX(0, F61- SUM(G61:H61))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K61">
-        <f>SUM(G61:H61)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3630,25 +3630,25 @@
         <v>295</v>
       </c>
       <c r="C62" s="3">
-        <f>LEN(A62)</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="D62" s="3">
         <v>280</v>
       </c>
       <c r="E62" t="str">
-        <f>CONCATENATE(B62,".",C62,".",D62,"    ",A62)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.16.280    on i skol dour  </v>
       </c>
       <c r="F62">
         <v>0</v>
       </c>
       <c r="I62">
-        <f>MAX(0, F62- SUM(G62:H62))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K62">
-        <f>SUM(G62:H62)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3660,14 +3660,14 @@
         <v>295</v>
       </c>
       <c r="C63" s="3">
-        <f>LEN(A63)</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="D63" s="3">
         <v>285</v>
       </c>
       <c r="E63" t="str">
-        <f>CONCATENATE(B63,".",C63,".",D63,"    ",A63)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.17.285    on ice cold our  </v>
       </c>
       <c r="F63">
@@ -3677,11 +3677,11 @@
         <v>0</v>
       </c>
       <c r="I63">
-        <f>MAX(0, F63- SUM(G63:H63))</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K63">
-        <f>SUM(G63:H63)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3693,25 +3693,25 @@
         <v>295</v>
       </c>
       <c r="C64" s="3">
-        <f>LEN(A64)</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="D64" s="3">
         <v>291</v>
       </c>
       <c r="E64" t="str">
-        <f>CONCATENATE(B64,".",C64,".",D64,"    ",A64)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.17.291    on ice-cold our  </v>
       </c>
       <c r="F64">
         <v>2</v>
       </c>
       <c r="I64">
-        <f>MAX(0, F64- SUM(G64:H64))</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K64">
-        <f>SUM(G64:H64)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3723,25 +3723,25 @@
         <v>295</v>
       </c>
       <c r="C65" s="3">
-        <f>LEN(A65)</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="D65" s="3">
         <v>70</v>
       </c>
       <c r="E65" t="str">
-        <f>CONCATENATE(B65,".",C65,".",D65,"    ",A65)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">A.17.70    a nye skol dour  </v>
       </c>
       <c r="F65">
         <v>0</v>
       </c>
       <c r="I65">
-        <f>MAX(0, F65- SUM(G65:H65))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K65">
-        <f>SUM(G65:H65)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3753,25 +3753,25 @@
         <v>295</v>
       </c>
       <c r="C66" s="3">
-        <f>LEN(A66)</f>
+        <f t="shared" ref="C66:C97" si="8">LEN(A66)</f>
         <v>18</v>
       </c>
       <c r="D66" s="3">
         <v>110</v>
       </c>
       <c r="E66" t="str">
-        <f>CONCATENATE(B66,".",C66,".",D66,"    ",A66)</f>
+        <f t="shared" ref="E66:E97" si="9">CONCATENATE(B66,".",C66,".",D66,"    ",A66)</f>
         <v xml:space="preserve">A.18.110    ah nye skol dour  </v>
       </c>
       <c r="F66">
         <v>0</v>
       </c>
       <c r="I66">
-        <f>MAX(0, F66- SUM(G66:H66))</f>
+        <f t="shared" ref="I66:I97" si="10">MAX(0, F66- SUM(G66:H66))</f>
         <v>0</v>
       </c>
       <c r="K66">
-        <f>SUM(G66:H66)</f>
+        <f t="shared" ref="K66:K97" si="11">SUM(G66:H66)</f>
         <v>0</v>
       </c>
     </row>
@@ -3783,25 +3783,25 @@
         <v>295</v>
       </c>
       <c r="C67" s="3">
-        <f>LEN(A67)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D67" s="3">
         <v>118</v>
       </c>
       <c r="E67" t="str">
-        <f>CONCATENATE(B67,".",C67,".",D67,"    ",A67)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.118    an aye skol dour  </v>
       </c>
       <c r="F67">
         <v>0</v>
       </c>
       <c r="I67">
-        <f>MAX(0, F67- SUM(G67:H67))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K67">
-        <f>SUM(G67:H67)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3813,25 +3813,25 @@
         <v>295</v>
       </c>
       <c r="C68" s="3">
-        <f>LEN(A68)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D68" s="3">
         <v>126</v>
       </c>
       <c r="E68" t="str">
-        <f>CONCATENATE(B68,".",C68,".",D68,"    ",A68)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.126    an eye skol dour  </v>
       </c>
       <c r="F68">
         <v>0</v>
       </c>
       <c r="I68">
-        <f>MAX(0, F68- SUM(G68:H68))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K68">
-        <f>SUM(G68:H68)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3843,25 +3843,25 @@
         <v>295</v>
       </c>
       <c r="C69" s="3">
-        <f>LEN(A69)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D69" s="3">
         <v>132</v>
       </c>
       <c r="E69" t="str">
-        <f>CONCATENATE(B69,".",C69,".",D69,"    ",A69)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.132    an ice coal dour  </v>
       </c>
       <c r="F69">
         <v>0</v>
       </c>
       <c r="I69">
-        <f>MAX(0, F69- SUM(G69:H69))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K69">
-        <f>SUM(G69:H69)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3873,25 +3873,25 @@
         <v>295</v>
       </c>
       <c r="C70" s="3">
-        <f>LEN(A70)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D70" s="3">
         <v>136</v>
       </c>
       <c r="E70" t="str">
-        <f>CONCATENATE(B70,".",C70,".",D70,"    ",A70)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.136    an ice cole dour  </v>
       </c>
       <c r="F70">
         <v>0</v>
       </c>
       <c r="I70">
-        <f>MAX(0, F70- SUM(G70:H70))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K70">
-        <f>SUM(G70:H70)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3903,25 +3903,25 @@
         <v>295</v>
       </c>
       <c r="C71" s="3">
-        <f>LEN(A71)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D71" s="3">
         <v>138</v>
       </c>
       <c r="E71" t="str">
-        <f>CONCATENATE(B71,".",C71,".",D71,"    ",A71)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.138    an ice kohl dour  </v>
       </c>
       <c r="F71">
         <v>0</v>
       </c>
       <c r="I71">
-        <f>MAX(0, F71- SUM(G71:H71))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K71">
-        <f>SUM(G71:H71)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3933,14 +3933,14 @@
         <v>295</v>
       </c>
       <c r="C72" s="3">
-        <f>LEN(A72)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D72" s="3">
         <v>161</v>
       </c>
       <c r="E72" t="str">
-        <f>CONCATENATE(B72,".",C72,".",D72,"    ",A72)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.161    eh nice cold our  </v>
       </c>
       <c r="F72">
@@ -3950,11 +3950,11 @@
         <v>0</v>
       </c>
       <c r="I72">
-        <f>MAX(0, F72- SUM(G72:H72))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="K72">
-        <f>SUM(G72:H72)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3966,25 +3966,25 @@
         <v>295</v>
       </c>
       <c r="C73" s="3">
-        <f>LEN(A73)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D73" s="3">
         <v>180</v>
       </c>
       <c r="E73" t="str">
-        <f>CONCATENATE(B73,".",C73,".",D73,"    ",A73)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.180    eh nye skol dour  </v>
       </c>
       <c r="F73">
         <v>0</v>
       </c>
       <c r="I73">
-        <f>MAX(0, F73- SUM(G73:H73))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K73">
-        <f>SUM(G73:H73)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3996,25 +3996,25 @@
         <v>295</v>
       </c>
       <c r="C74" s="3">
-        <f>LEN(A74)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D74" s="3">
         <v>268</v>
       </c>
       <c r="E74" t="str">
-        <f>CONCATENATE(B74,".",C74,".",D74,"    ",A74)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.268    on aye skol dour  </v>
       </c>
       <c r="F74">
         <v>0</v>
       </c>
       <c r="I74">
-        <f>MAX(0, F74- SUM(G74:H74))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K74">
-        <f>SUM(G74:H74)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4026,25 +4026,25 @@
         <v>295</v>
       </c>
       <c r="C75" s="3">
-        <f>LEN(A75)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D75" s="3">
         <v>276</v>
       </c>
       <c r="E75" t="str">
-        <f>CONCATENATE(B75,".",C75,".",D75,"    ",A75)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.276    on eye skol dour  </v>
       </c>
       <c r="F75">
         <v>0</v>
       </c>
       <c r="I75">
-        <f>MAX(0, F75- SUM(G75:H75))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K75">
-        <f>SUM(G75:H75)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4056,25 +4056,25 @@
         <v>295</v>
       </c>
       <c r="C76" s="3">
-        <f>LEN(A76)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D76" s="3">
         <v>282</v>
       </c>
       <c r="E76" t="str">
-        <f>CONCATENATE(B76,".",C76,".",D76,"    ",A76)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.282    on ice coal dour  </v>
       </c>
       <c r="F76">
         <v>0</v>
       </c>
       <c r="I76">
-        <f>MAX(0, F76- SUM(G76:H76))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K76">
-        <f>SUM(G76:H76)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4086,25 +4086,25 @@
         <v>295</v>
       </c>
       <c r="C77" s="3">
-        <f>LEN(A77)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D77" s="3">
         <v>286</v>
       </c>
       <c r="E77" t="str">
-        <f>CONCATENATE(B77,".",C77,".",D77,"    ",A77)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.286    on ice cole dour  </v>
       </c>
       <c r="F77">
         <v>0</v>
       </c>
       <c r="I77">
-        <f>MAX(0, F77- SUM(G77:H77))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K77">
-        <f>SUM(G77:H77)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4116,25 +4116,25 @@
         <v>295</v>
       </c>
       <c r="C78" s="3">
-        <f>LEN(A78)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D78" s="3">
         <v>288</v>
       </c>
       <c r="E78" t="str">
-        <f>CONCATENATE(B78,".",C78,".",D78,"    ",A78)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.288    on ice kohl dour  </v>
       </c>
       <c r="F78">
         <v>0</v>
       </c>
       <c r="I78">
-        <f>MAX(0, F78- SUM(G78:H78))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K78">
-        <f>SUM(G78:H78)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4146,25 +4146,25 @@
         <v>295</v>
       </c>
       <c r="C79" s="3">
-        <f>LEN(A79)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D79" s="3">
         <v>48</v>
       </c>
       <c r="E79" t="str">
-        <f>CONCATENATE(B79,".",C79,".",D79,"    ",A79)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.48    a nice coal dour  </v>
       </c>
       <c r="F79">
         <v>0</v>
       </c>
       <c r="I79">
-        <f>MAX(0, F79- SUM(G79:H79))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K79">
-        <f>SUM(G79:H79)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4176,14 +4176,14 @@
         <v>295</v>
       </c>
       <c r="C80" s="3">
-        <f>LEN(A80)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D80" s="3">
         <v>50</v>
       </c>
       <c r="E80" t="str">
-        <f>CONCATENATE(B80,".",C80,".",D80,"    ",A80)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.50    a nice cold hour  </v>
       </c>
       <c r="F80">
@@ -4193,11 +4193,11 @@
         <v>0</v>
       </c>
       <c r="I80">
-        <f>MAX(0, F80- SUM(G80:H80))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="K80">
-        <f>SUM(G80:H80)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4209,25 +4209,25 @@
         <v>295</v>
       </c>
       <c r="C81" s="3">
-        <f>LEN(A81)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D81" s="3">
         <v>52</v>
       </c>
       <c r="E81" t="str">
-        <f>CONCATENATE(B81,".",C81,".",D81,"    ",A81)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.52    a nice cole dour  </v>
       </c>
       <c r="F81">
         <v>0</v>
       </c>
       <c r="I81">
-        <f>MAX(0, F81- SUM(G81:H81))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K81">
-        <f>SUM(G81:H81)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4239,25 +4239,25 @@
         <v>295</v>
       </c>
       <c r="C82" s="3">
-        <f>LEN(A82)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D82" s="3">
         <v>54</v>
       </c>
       <c r="E82" t="str">
-        <f>CONCATENATE(B82,".",C82,".",D82,"    ",A82)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.54    a nice kohl dour  </v>
       </c>
       <c r="F82">
         <v>0</v>
       </c>
       <c r="I82">
-        <f>MAX(0, F82- SUM(G82:H82))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K82">
-        <f>SUM(G82:H82)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4269,25 +4269,25 @@
         <v>295</v>
       </c>
       <c r="C83" s="3">
-        <f>LEN(A83)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="D83" s="3">
         <v>66</v>
       </c>
       <c r="E83" t="str">
-        <f>CONCATENATE(B83,".",C83,".",D83,"    ",A83)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.18.66    a nigh skol dour  </v>
       </c>
       <c r="F83">
         <v>0</v>
       </c>
       <c r="I83">
-        <f>MAX(0, F83- SUM(G83:H83))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K83">
-        <f>SUM(G83:H83)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4299,25 +4299,25 @@
         <v>295</v>
       </c>
       <c r="C84" s="3">
-        <f>LEN(A84)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D84" s="3">
         <v>106</v>
       </c>
       <c r="E84" t="str">
-        <f>CONCATENATE(B84,".",C84,".",D84,"    ",A84)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.106    ah nigh skol dour  </v>
       </c>
       <c r="F84">
         <v>0</v>
       </c>
       <c r="I84">
-        <f>MAX(0, F84- SUM(G84:H84))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K84">
-        <f>SUM(G84:H84)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4329,14 +4329,14 @@
         <v>295</v>
       </c>
       <c r="C85" s="3">
-        <f>LEN(A85)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D85" s="3">
         <v>124</v>
       </c>
       <c r="E85" t="str">
-        <f>CONCATENATE(B85,".",C85,".",D85,"    ",A85)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.124    an eye scold hour  </v>
       </c>
       <c r="F85">
@@ -4346,11 +4346,11 @@
         <v>0</v>
       </c>
       <c r="I85">
-        <f>MAX(0, F85- SUM(G85:H85))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="K85">
-        <f>SUM(G85:H85)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4362,14 +4362,14 @@
         <v>295</v>
       </c>
       <c r="C86" s="3">
-        <f>LEN(A86)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D86" s="3">
         <v>137</v>
       </c>
       <c r="E86" t="str">
-        <f>CONCATENATE(B86,".",C86,".",D86,"    ",A86)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.137    an ice cole dower  </v>
       </c>
       <c r="F86">
@@ -4379,11 +4379,11 @@
         <v>0</v>
       </c>
       <c r="I86">
-        <f>MAX(0, F86- SUM(G86:H86))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="K86">
-        <f>SUM(G86:H86)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4395,25 +4395,25 @@
         <v>295</v>
       </c>
       <c r="C87" s="3">
-        <f>LEN(A87)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D87" s="3">
         <v>158</v>
       </c>
       <c r="E87" t="str">
-        <f>CONCATENATE(B87,".",C87,".",D87,"    ",A87)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.158    eh nice coal dour  </v>
       </c>
       <c r="F87">
         <v>0</v>
       </c>
       <c r="I87">
-        <f>MAX(0, F87- SUM(G87:H87))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K87">
-        <f>SUM(G87:H87)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4425,25 +4425,25 @@
         <v>295</v>
       </c>
       <c r="C88" s="3">
-        <f>LEN(A88)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D88" s="3">
         <v>162</v>
       </c>
       <c r="E88" t="str">
-        <f>CONCATENATE(B88,".",C88,".",D88,"    ",A88)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.162    eh nice cole dour  </v>
       </c>
       <c r="F88">
         <v>0</v>
       </c>
       <c r="I88">
-        <f>MAX(0, F88- SUM(G88:H88))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K88">
-        <f>SUM(G88:H88)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4455,25 +4455,25 @@
         <v>295</v>
       </c>
       <c r="C89" s="3">
-        <f>LEN(A89)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D89" s="3">
         <v>164</v>
       </c>
       <c r="E89" t="str">
-        <f>CONCATENATE(B89,".",C89,".",D89,"    ",A89)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.164    eh nice kohl dour  </v>
       </c>
       <c r="F89">
         <v>0</v>
       </c>
       <c r="I89">
-        <f>MAX(0, F89- SUM(G89:H89))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K89">
-        <f>SUM(G89:H89)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4485,25 +4485,25 @@
         <v>295</v>
       </c>
       <c r="C90" s="3">
-        <f>LEN(A90)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D90" s="3">
         <v>176</v>
       </c>
       <c r="E90" t="str">
-        <f>CONCATENATE(B90,".",C90,".",D90,"    ",A90)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.176    eh nigh skol dour  </v>
       </c>
       <c r="F90">
         <v>0</v>
       </c>
       <c r="I90">
-        <f>MAX(0, F90- SUM(G90:H90))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K90">
-        <f>SUM(G90:H90)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4515,14 +4515,14 @@
         <v>295</v>
       </c>
       <c r="C91" s="3">
-        <f>LEN(A91)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D91" s="3">
         <v>178</v>
       </c>
       <c r="E91" t="str">
-        <f>CONCATENATE(B91,".",C91,".",D91,"    ",A91)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.178    eh nye scold hour  </v>
       </c>
       <c r="F91">
@@ -4532,11 +4532,11 @@
         <v>0</v>
       </c>
       <c r="I91">
-        <f>MAX(0, F91- SUM(G91:H91))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="K91">
-        <f>SUM(G91:H91)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4548,14 +4548,14 @@
         <v>295</v>
       </c>
       <c r="C92" s="3">
-        <f>LEN(A92)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D92" s="3">
         <v>277</v>
       </c>
       <c r="E92" t="str">
-        <f>CONCATENATE(B92,".",C92,".",D92,"    ",A92)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.277    on eye skol dower  </v>
       </c>
       <c r="F92">
@@ -4565,11 +4565,11 @@
         <v>0</v>
       </c>
       <c r="I92">
-        <f>MAX(0, F92- SUM(G92:H92))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="K92">
-        <f>SUM(G92:H92)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4581,14 +4581,14 @@
         <v>295</v>
       </c>
       <c r="C93" s="3">
-        <f>LEN(A93)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D93" s="3">
         <v>287</v>
       </c>
       <c r="E93" t="str">
-        <f>CONCATENATE(B93,".",C93,".",D93,"    ",A93)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.287    on ice cole dower  </v>
       </c>
       <c r="F93">
@@ -4598,11 +4598,11 @@
         <v>0</v>
       </c>
       <c r="I93">
-        <f>MAX(0, F93- SUM(G93:H93))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="K93">
-        <f>SUM(G93:H93)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4614,25 +4614,25 @@
         <v>295</v>
       </c>
       <c r="C94" s="3">
-        <f>LEN(A94)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D94" s="3">
         <v>53</v>
       </c>
       <c r="E94" t="str">
-        <f>CONCATENATE(B94,".",C94,".",D94,"    ",A94)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.53    a nice cole dower  </v>
       </c>
       <c r="F94">
         <v>2</v>
       </c>
       <c r="I94">
-        <f>MAX(0, F94- SUM(G94:H94))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="K94">
-        <f>SUM(G94:H94)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4644,25 +4644,25 @@
         <v>295</v>
       </c>
       <c r="C95" s="3">
-        <f>LEN(A95)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D95" s="3">
         <v>55</v>
       </c>
       <c r="E95" t="str">
-        <f>CONCATENATE(B95,".",C95,".",D95,"    ",A95)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.55    a nice kohl dower  </v>
       </c>
       <c r="F95">
         <v>2</v>
       </c>
       <c r="I95">
-        <f>MAX(0, F95- SUM(G95:H95))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="K95">
-        <f>SUM(G95:H95)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4674,14 +4674,14 @@
         <v>295</v>
       </c>
       <c r="C96" s="3">
-        <f>LEN(A96)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D96" s="3">
         <v>67</v>
       </c>
       <c r="E96" t="str">
-        <f>CONCATENATE(B96,".",C96,".",D96,"    ",A96)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.67    a nigh skol dower  </v>
       </c>
       <c r="F96">
@@ -4691,11 +4691,11 @@
         <v>0</v>
       </c>
       <c r="I96">
-        <f>MAX(0, F96- SUM(G96:H96))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="K96">
-        <f>SUM(G96:H96)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4707,25 +4707,25 @@
         <v>295</v>
       </c>
       <c r="C97" s="3">
-        <f>LEN(A97)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="D97" s="3">
         <v>88</v>
       </c>
       <c r="E97" t="str">
-        <f>CONCATENATE(B97,".",C97,".",D97,"    ",A97)</f>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">A.19.88    ah nice coal dour  </v>
       </c>
       <c r="F97">
         <v>0</v>
       </c>
       <c r="I97">
-        <f>MAX(0, F97- SUM(G97:H97))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K97">
-        <f>SUM(G97:H97)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -4737,25 +4737,25 @@
         <v>295</v>
       </c>
       <c r="C98" s="3">
-        <f>LEN(A98)</f>
+        <f t="shared" ref="C98:C106" si="12">LEN(A98)</f>
         <v>19</v>
       </c>
       <c r="D98" s="3">
         <v>92</v>
       </c>
       <c r="E98" t="str">
-        <f>CONCATENATE(B98,".",C98,".",D98,"    ",A98)</f>
+        <f t="shared" ref="E98:E106" si="13">CONCATENATE(B98,".",C98,".",D98,"    ",A98)</f>
         <v xml:space="preserve">A.19.92    ah nice cole dour  </v>
       </c>
       <c r="F98">
         <v>0</v>
       </c>
       <c r="I98">
-        <f>MAX(0, F98- SUM(G98:H98))</f>
+        <f t="shared" ref="I98:I106" si="14">MAX(0, F98- SUM(G98:H98))</f>
         <v>0</v>
       </c>
       <c r="K98">
-        <f>SUM(G98:H98)</f>
+        <f t="shared" ref="K98:K106" si="15">SUM(G98:H98)</f>
         <v>0</v>
       </c>
     </row>
@@ -4767,25 +4767,25 @@
         <v>295</v>
       </c>
       <c r="C99" s="3">
-        <f>LEN(A99)</f>
+        <f t="shared" si="12"/>
         <v>19</v>
       </c>
       <c r="D99" s="3">
         <v>94</v>
       </c>
       <c r="E99" t="str">
-        <f>CONCATENATE(B99,".",C99,".",D99,"    ",A99)</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">A.19.94    ah nice kohl dour  </v>
       </c>
       <c r="F99">
         <v>0</v>
       </c>
       <c r="I99">
-        <f>MAX(0, F99- SUM(G99:H99))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K99">
-        <f>SUM(G99:H99)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4797,14 +4797,14 @@
         <v>295</v>
       </c>
       <c r="C100" s="3">
-        <f>LEN(A100)</f>
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
       <c r="D100" s="3">
         <v>104</v>
       </c>
       <c r="E100" t="str">
-        <f>CONCATENATE(B100,".",C100,".",D100,"    ",A100)</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">A.20.104    ah nigh scold hour  </v>
       </c>
       <c r="F100">
@@ -4814,11 +4814,11 @@
         <v>0</v>
       </c>
       <c r="I100">
-        <f>MAX(0, F100- SUM(G100:H100))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="K100">
-        <f>SUM(G100:H100)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4830,14 +4830,14 @@
         <v>295</v>
       </c>
       <c r="C101" s="3">
-        <f>LEN(A101)</f>
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
       <c r="D101" s="3">
         <v>107</v>
       </c>
       <c r="E101" t="str">
-        <f>CONCATENATE(B101,".",C101,".",D101,"    ",A101)</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">A.20.107    ah nigh skol dower  </v>
       </c>
       <c r="F101">
@@ -4847,11 +4847,11 @@
         <v>0</v>
       </c>
       <c r="I101">
-        <f>MAX(0, F101- SUM(G101:H101))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="K101">
-        <f>SUM(G101:H101)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4863,14 +4863,14 @@
         <v>295</v>
       </c>
       <c r="C102" s="3">
-        <f>LEN(A102)</f>
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
       <c r="D102" s="3">
         <v>165</v>
       </c>
       <c r="E102" t="str">
-        <f>CONCATENATE(B102,".",C102,".",D102,"    ",A102)</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">A.20.165    eh nice kohl dower  </v>
       </c>
       <c r="F102">
@@ -4880,11 +4880,11 @@
         <v>0</v>
       </c>
       <c r="I102">
-        <f>MAX(0, F102- SUM(G102:H102))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="K102">
-        <f>SUM(G102:H102)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4896,14 +4896,14 @@
         <v>296</v>
       </c>
       <c r="C103" s="3">
-        <f>LEN(A103)</f>
+        <f t="shared" si="12"/>
         <v>15</v>
       </c>
       <c r="D103" s="3">
         <v>14</v>
       </c>
       <c r="E103" t="str">
-        <f>CONCATENATE(B103,".",C103,".",D103,"    ",A103)</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">B.15.14    fourth rye to  </v>
       </c>
       <c r="F103">
@@ -4913,11 +4913,11 @@
         <v>0</v>
       </c>
       <c r="I103">
-        <f>MAX(0, F103- SUM(G103:H103))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="K103">
-        <f>SUM(G103:H103)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4929,14 +4929,14 @@
         <v>296</v>
       </c>
       <c r="C104" s="3">
-        <f>LEN(A104)</f>
+        <f t="shared" si="12"/>
         <v>16</v>
       </c>
       <c r="D104" s="3">
         <v>11</v>
       </c>
       <c r="E104" t="str">
-        <f>CONCATENATE(B104,".",C104,".",D104,"    ",A104)</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">B.16.11    forthright ooh  </v>
       </c>
       <c r="F104">
@@ -4946,11 +4946,11 @@
         <v>0</v>
       </c>
       <c r="I104">
-        <f>MAX(0, F104- SUM(G104:H104))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="K104">
-        <f>SUM(G104:H104)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4962,14 +4962,14 @@
         <v>296</v>
       </c>
       <c r="C105" s="3">
-        <f>LEN(A105)</f>
+        <f t="shared" si="12"/>
         <v>16</v>
       </c>
       <c r="D105" s="3">
         <v>21</v>
       </c>
       <c r="E105" t="str">
-        <f>CONCATENATE(B105,".",C105,".",D105,"    ",A105)</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">B.16.21    fourth wry two  </v>
       </c>
       <c r="F105">
@@ -4979,11 +4979,11 @@
         <v>0</v>
       </c>
       <c r="I105">
-        <f>MAX(0, F105- SUM(G105:H105))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="K105">
-        <f>SUM(G105:H105)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4995,14 +4995,14 @@
         <v>296</v>
       </c>
       <c r="C106" s="3">
-        <f>LEN(A106)</f>
+        <f t="shared" si="12"/>
         <v>18</v>
       </c>
       <c r="D106" s="3">
         <v>18</v>
       </c>
       <c r="E106" t="str">
-        <f>CONCATENATE(B106,".",C106,".",D106,"    ",A106)</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">B.18.18    fourth write ooh  </v>
       </c>
       <c r="F106">
@@ -5012,11 +5012,11 @@
         <v>0</v>
       </c>
       <c r="I106">
-        <f>MAX(0, F106- SUM(G106:H106))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="K106">
-        <f>SUM(G106:H106)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -5039,7 +5039,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -9278,7 +9277,7 @@
         <v>34</v>
       </c>
       <c r="E194" t="str">
-        <f t="shared" ref="E194:E257" si="7">CONCATENATE(B194,".",C194,".",D194,"    ",A194)</f>
+        <f t="shared" ref="E194:E207" si="7">CONCATENATE(B194,".",C194,".",D194,"    ",A194)</f>
         <v xml:space="preserve">A.20.34    a gneiss cold hour  </v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new country breakdown pie charts
</commit_message>
<xml_diff>
--- a/MechanicalTurkStuff/PhrasesToRead.xlsx
+++ b/MechanicalTurkStuff/PhrasesToRead.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="9440" yWindow="1960" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="329">
   <si>
     <t>orthoPhrase</t>
   </si>
@@ -998,6 +998,18 @@
   </si>
   <si>
     <t>Total recordings</t>
+  </si>
+  <si>
+    <t>PHRASE A</t>
+  </si>
+  <si>
+    <t>PHRASE B</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -1589,10 +1601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K106"/>
+  <dimension ref="A1:L109"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="J109" sqref="J109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1638,225 +1650,216 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C2" s="3">
-        <f t="shared" ref="C2:C33" si="0">LEN(A2)</f>
-        <v>17</v>
+        <f>LEN(A2)</f>
+        <v>16</v>
       </c>
       <c r="D2" s="3">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E33" si="1">CONCATENATE(B2,".",C2,".",D2,"    ",A2)</f>
-        <v xml:space="preserve">A.17.51    a nice cold our  </v>
+        <f>CONCATENATE(B2,".",C2,".",D2,"    ",A2)</f>
+        <v xml:space="preserve">A.16.129    an i scold our  </v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
       <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I33" si="2">MAX(0, F2- SUM(G2:H2))</f>
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>319</v>
+        <f>MAX(0, F2- SUM(G2:H2))</f>
+        <v>2</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K33" si="3">SUM(G2:H2)</f>
-        <v>3</v>
+        <f>SUM(G2:H2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>LEN(A3)</f>
+        <v>16</v>
       </c>
       <c r="D3" s="3">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.17.135    an ice cold our  </v>
+        <f>CONCATENATE(B3,".",C3,".",D3,"    ",A3)</f>
+        <v xml:space="preserve">A.16.130    an i skol dour  </v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" si="2"/>
+        <f>MAX(0, F3- SUM(G3:H3))</f>
         <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G3:H3)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>278</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>LEN(A4)</f>
+        <v>16</v>
       </c>
       <c r="D4" s="3">
-        <v>69</v>
+        <v>279</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.17.69    a nye scold our  </v>
+        <f>CONCATENATE(B4,".",C4,".",D4,"    ",A4)</f>
+        <v xml:space="preserve">A.16.279    on i scold our  </v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, F4- SUM(G4:H4))</f>
+        <v>1</v>
       </c>
       <c r="K4">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G4:H4)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>279</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f>LEN(A5)</f>
+        <v>16</v>
       </c>
       <c r="D5" s="3">
-        <v>109</v>
+        <v>280</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.18.109    ah nye scold our  </v>
+        <f>CONCATENATE(B5,".",C5,".",D5,"    ",A5)</f>
+        <v xml:space="preserve">A.16.280    on i skol dour  </v>
       </c>
       <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f>MAX(0, F5- SUM(G5:H5))</f>
         <v>0</v>
       </c>
       <c r="K5">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G5:H5)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f>LEN(A6)</f>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.18.125    an eye scold our  </v>
+        <f>CONCATENATE(B6,".",C6,".",D6,"    ",A6)</f>
+        <v xml:space="preserve">A.17.128    an i scold hour  </v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, F6- SUM(G6:H6))</f>
+        <v>2</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G6:H6)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>266</v>
+        <v>130</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f>LEN(A7)</f>
+        <v>17</v>
       </c>
       <c r="D7" s="3">
-        <v>267</v>
+        <v>131</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.18.267    on aye scold our  </v>
+        <f>CONCATENATE(B7,".",C7,".",D7,"    ",A7)</f>
+        <v xml:space="preserve">A.17.131    an i skol dower  </v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, F7- SUM(G7:H7))</f>
+        <v>1</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G7:H7)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f>LEN(A8)</f>
+        <v>17</v>
       </c>
       <c r="D8" s="3">
-        <v>65</v>
+        <v>135</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.18.65    a nigh scold our  </v>
+        <f>CONCATENATE(B8,".",C8,".",D8,"    ",A8)</f>
+        <v xml:space="preserve">A.17.135    an ice cold our  </v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -1865,196 +1868,193 @@
         <v>2</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f>MAX(0, F8- SUM(G8:H8))</f>
         <v>0</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
+        <f>SUM(G8:H8)</f>
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f>LEN(A9)</f>
+        <v>17</v>
       </c>
       <c r="D9" s="3">
-        <v>71</v>
+        <v>141</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.18.71    a nye skol dower  </v>
+        <f>CONCATENATE(B9,".",C9,".",D9,"    ",A9)</f>
+        <v xml:space="preserve">A.17.141    an ice-cold our  </v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, F9- SUM(G9:H9))</f>
+        <v>1</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G9:H9)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <f>LEN(A10)</f>
+        <v>17</v>
       </c>
       <c r="D10" s="3">
-        <v>119</v>
+        <v>278</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.19.119    an aye skol dower  </v>
+        <f>CONCATENATE(B10,".",C10,".",D10,"    ",A10)</f>
+        <v xml:space="preserve">A.17.278    on i scold hour  </v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, F10- SUM(G10:H10))</f>
+        <v>1</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G10:H10)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>280</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <f>LEN(A11)</f>
+        <v>17</v>
       </c>
       <c r="D11" s="3">
-        <v>127</v>
+        <v>281</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.19.127    an eye skol dower  </v>
+        <f>CONCATENATE(B11,".",C11,".",D11,"    ",A11)</f>
+        <v xml:space="preserve">A.17.281    on i skol dower  </v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, F11- SUM(G11:H11))</f>
+        <v>1</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G11:H11)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>284</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <f>LEN(A12)</f>
+        <v>17</v>
       </c>
       <c r="D12" s="3">
-        <v>133</v>
+        <v>285</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.19.133    an ice coal dower  </v>
+        <f>CONCATENATE(B12,".",C12,".",D12,"    ",A12)</f>
+        <v xml:space="preserve">A.17.285    on ice cold our  </v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, F12- SUM(G12:H12))</f>
+        <v>2</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G12:H12)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>290</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>LEN(A13)</f>
+        <v>17</v>
       </c>
       <c r="D13" s="3">
-        <v>159</v>
+        <v>291</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.20.159    eh nice coal dower  </v>
+        <f>CONCATENATE(B13,".",C13,".",D13,"    ",A13)</f>
+        <v xml:space="preserve">A.17.291    on ice-cold our  </v>
       </c>
       <c r="F13">
-        <v>3</v>
-      </c>
-      <c r="G13">
         <v>2</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>MAX(0, F13- SUM(G13:H13))</f>
+        <v>2</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G13:H13)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>LEN(A14)</f>
+        <v>17</v>
       </c>
       <c r="D14" s="3">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.20.89    ah nice coal dower  </v>
+        <f>CONCATENATE(B14,".",C14,".",D14,"    ",A14)</f>
+        <v xml:space="preserve">A.17.51    a nice cold our  </v>
       </c>
       <c r="F14">
         <v>2</v>
@@ -2062,32 +2062,38 @@
       <c r="G14">
         <v>2</v>
       </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
       <c r="I14">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, F14- SUM(G14:H14))</f>
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>319</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G14:H14)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>315</v>
-      </c>
-      <c r="B15" t="s">
-        <v>296</v>
+        <v>68</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f>LEN(A15)</f>
+        <v>17</v>
       </c>
       <c r="D15" s="3">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">B.15.19    fourth wry to  </v>
+        <f>CONCATENATE(B15,".",C15,".",D15,"    ",A15)</f>
+        <v xml:space="preserve">A.17.69    a nye scold our  </v>
       </c>
       <c r="F15">
         <v>2</v>
@@ -2096,64 +2102,61 @@
         <v>2</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f>MAX(0, F15- SUM(G15:H15))</f>
         <v>0</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
+        <f>SUM(G15:H15)</f>
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>316</v>
-      </c>
-      <c r="B16" t="s">
-        <v>296</v>
+        <v>69</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>295</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f>LEN(A16)</f>
+        <v>17</v>
       </c>
       <c r="D16" s="3">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">B.16.20    fourth wry too  </v>
+        <f>CONCATENATE(B16,".",C16,".",D16,"    ",A16)</f>
+        <v xml:space="preserve">A.17.70    a nye skol dour  </v>
       </c>
       <c r="F16">
-        <v>2</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
+        <f>MAX(0, F16- SUM(G16:H16))</f>
         <v>0</v>
       </c>
       <c r="K16">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G16:H16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>297</v>
-      </c>
-      <c r="B17" t="s">
-        <v>296</v>
+        <v>108</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>LEN(A17)</f>
+        <v>18</v>
       </c>
       <c r="D17" s="3">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">B.17.1    forth right ooh  </v>
+        <f>CONCATENATE(B17,".",C17,".",D17,"    ",A17)</f>
+        <v xml:space="preserve">A.18.109    ah nye scold our  </v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -2162,375 +2165,357 @@
         <v>2</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
+        <f>MAX(0, F17- SUM(G17:H17))</f>
         <v>0</v>
       </c>
       <c r="K17">
-        <f t="shared" si="3"/>
+        <f>SUM(G17:H17)</f>
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>309</v>
-      </c>
-      <c r="B18" t="s">
-        <v>296</v>
+        <v>109</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>295</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>LEN(A18)</f>
+        <v>18</v>
       </c>
       <c r="D18" s="3">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">B.17.13    fourth rite ooh  </v>
+        <f>CONCATENATE(B18,".",C18,".",D18,"    ",A18)</f>
+        <v xml:space="preserve">A.18.110    ah nye skol dour  </v>
       </c>
       <c r="F18">
-        <v>2</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f>MAX(0, F18- SUM(G18:H18))</f>
         <v>0</v>
       </c>
       <c r="K18">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G18:H18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>302</v>
-      </c>
-      <c r="B19" t="s">
-        <v>296</v>
+        <v>116</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" si="0"/>
+        <f>LEN(A19)</f>
         <v>18</v>
       </c>
       <c r="D19" s="3">
-        <v>6</v>
+        <v>117</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">B.18.6    forth wright ooh  </v>
+        <f>CONCATENATE(B19,".",C19,".",D19,"    ",A19)</f>
+        <v xml:space="preserve">A.18.117    an aye scold our  </v>
       </c>
       <c r="F19">
         <v>2</v>
       </c>
       <c r="G19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MAX(0, F19- SUM(G19:H19))</f>
+        <v>1</v>
       </c>
       <c r="K19">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f>SUM(G19:H19)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>278</v>
-      </c>
-      <c r="B20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f>LEN(A20)</f>
+        <v>18</v>
       </c>
       <c r="D20" s="3">
-        <v>279</v>
+        <v>118</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.16.279    on i scold our  </v>
+        <f>CONCATENATE(B20,".",C20,".",D20,"    ",A20)</f>
+        <v xml:space="preserve">A.18.118    an aye skol dour  </v>
       </c>
       <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>MAX(0, F20- SUM(G20:H20))</f>
+        <v>0</v>
       </c>
       <c r="K20">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>SUM(G20:H20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>LEN(A21)</f>
+        <v>18</v>
       </c>
       <c r="D21" s="3">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.17.128    an i scold hour  </v>
+        <f>CONCATENATE(B21,".",C21,".",D21,"    ",A21)</f>
+        <v xml:space="preserve">A.18.125    an eye scold our  </v>
       </c>
       <c r="F21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I21">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f>MAX(0, F21- SUM(G21:H21))</f>
+        <v>0</v>
       </c>
       <c r="K21">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>SUM(G21:H21)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>LEN(A22)</f>
+        <v>18</v>
       </c>
       <c r="D22" s="3">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.17.131    an i skol dower  </v>
+        <f>CONCATENATE(B22,".",C22,".",D22,"    ",A22)</f>
+        <v xml:space="preserve">A.18.126    an eye skol dour  </v>
       </c>
       <c r="F22">
-        <v>2</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>MAX(0, F22- SUM(G22:H22))</f>
+        <v>0</v>
       </c>
       <c r="K22">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>SUM(G22:H22)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>LEN(A23)</f>
+        <v>18</v>
       </c>
       <c r="D23" s="3">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.17.141    an ice-cold our  </v>
+        <f>CONCATENATE(B23,".",C23,".",D23,"    ",A23)</f>
+        <v xml:space="preserve">A.18.132    an ice coal dour  </v>
       </c>
       <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>MAX(0, F23- SUM(G23:H23))</f>
+        <v>0</v>
       </c>
       <c r="K23">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>SUM(G23:H23)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>277</v>
+        <v>133</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C24" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>LEN(A24)</f>
+        <v>18</v>
       </c>
       <c r="D24" s="3">
-        <v>278</v>
+        <v>134</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.17.278    on i scold hour  </v>
+        <f>CONCATENATE(B24,".",C24,".",D24,"    ",A24)</f>
+        <v xml:space="preserve">A.18.134    an ice cold hour  </v>
       </c>
       <c r="F24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
       <c r="I24">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>MAX(0, F24- SUM(G24:H24))</f>
+        <v>3</v>
       </c>
       <c r="K24">
-        <f t="shared" si="3"/>
+        <f>SUM(G24:H24)</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>280</v>
+        <v>135</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <f>LEN(A25)</f>
+        <v>18</v>
       </c>
       <c r="D25" s="3">
-        <v>281</v>
+        <v>136</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.17.281    on i skol dower  </v>
+        <f>CONCATENATE(B25,".",C25,".",D25,"    ",A25)</f>
+        <v xml:space="preserve">A.18.136    an ice cole dour  </v>
       </c>
       <c r="F25">
-        <v>2</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>MAX(0, F25- SUM(G25:H25))</f>
+        <v>0</v>
       </c>
       <c r="K25">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>SUM(G25:H25)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>116</v>
-      </c>
-      <c r="B26" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C26" s="3">
-        <f t="shared" si="0"/>
+        <f>LEN(A26)</f>
         <v>18</v>
       </c>
       <c r="D26" s="3">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.18.117    an aye scold our  </v>
+        <f>CONCATENATE(B26,".",C26,".",D26,"    ",A26)</f>
+        <v xml:space="preserve">A.18.138    an ice kohl dour  </v>
       </c>
       <c r="F26">
-        <v>2</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>MAX(0, F26- SUM(G26:H26))</f>
+        <v>0</v>
       </c>
       <c r="K26">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>SUM(G26:H26)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>133</v>
-      </c>
-      <c r="B27" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C27" s="3">
-        <f t="shared" si="0"/>
+        <f>LEN(A27)</f>
         <v>18</v>
       </c>
       <c r="D27" s="3">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.18.134    an ice cold hour  </v>
+        <f>CONCATENATE(B27,".",C27,".",D27,"    ",A27)</f>
+        <v xml:space="preserve">A.18.140    an ice-cold hour  </v>
       </c>
       <c r="F27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="I27">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f>MAX(0, F27- SUM(G27:H27))</f>
+        <v>1</v>
       </c>
       <c r="K27">
-        <f t="shared" si="3"/>
+        <f>SUM(G27:H27)</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C28" s="3">
-        <f t="shared" si="0"/>
+        <f>LEN(A28)</f>
         <v>18</v>
       </c>
       <c r="D28" s="3">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.18.140    an ice-cold hour  </v>
+        <f>CONCATENATE(B28,".",C28,".",D28,"    ",A28)</f>
+        <v xml:space="preserve">A.18.161    eh nice cold our  </v>
       </c>
       <c r="F28">
         <v>2</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>MAX(0, F28- SUM(G28:H28))</f>
+        <v>2</v>
       </c>
       <c r="K28">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>SUM(G28:H28)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2541,14 +2526,14 @@
         <v>295</v>
       </c>
       <c r="C29" s="3">
-        <f t="shared" si="0"/>
+        <f>LEN(A29)</f>
         <v>18</v>
       </c>
       <c r="D29" s="3">
         <v>179</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE(B29,".",C29,".",D29,"    ",A29)</f>
         <v xml:space="preserve">A.18.179    eh nye scold our  </v>
       </c>
       <c r="F29">
@@ -2558,130 +2543,124 @@
         <v>1</v>
       </c>
       <c r="I29">
-        <f t="shared" si="2"/>
+        <f>MAX(0, F29- SUM(G29:H29))</f>
         <v>1</v>
       </c>
       <c r="K29">
-        <f t="shared" si="3"/>
+        <f>SUM(G29:H29)</f>
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>274</v>
+        <v>179</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C30" s="3">
-        <f t="shared" si="0"/>
+        <f>LEN(A30)</f>
         <v>18</v>
       </c>
       <c r="D30" s="3">
-        <v>275</v>
+        <v>180</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.18.275    on eye scold our  </v>
+        <f>CONCATENATE(B30,".",C30,".",D30,"    ",A30)</f>
+        <v xml:space="preserve">A.18.180    eh nye skol dour  </v>
       </c>
       <c r="F30">
-        <v>2</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>MAX(0, F30- SUM(G30:H30))</f>
+        <v>0</v>
       </c>
       <c r="K30">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>SUM(G30:H30)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C31" s="3">
-        <f t="shared" si="0"/>
+        <f>LEN(A31)</f>
         <v>18</v>
       </c>
       <c r="D31" s="3">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.18.284    on ice cold hour  </v>
+        <f>CONCATENATE(B31,".",C31,".",D31,"    ",A31)</f>
+        <v xml:space="preserve">A.18.267    on aye scold our  </v>
       </c>
       <c r="F31">
         <v>2</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I31">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>MAX(0, F31- SUM(G31:H31))</f>
+        <v>0</v>
       </c>
       <c r="K31">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>SUM(G31:H31)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>289</v>
-      </c>
-      <c r="B32" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C32" s="3">
-        <f t="shared" si="0"/>
+        <f>LEN(A32)</f>
         <v>18</v>
       </c>
       <c r="D32" s="3">
-        <v>290</v>
+        <v>268</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.18.290    on ice-cold hour  </v>
+        <f>CONCATENATE(B32,".",C32,".",D32,"    ",A32)</f>
+        <v xml:space="preserve">A.18.268    on aye skol dour  </v>
       </c>
       <c r="F32">
-        <v>2</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>MAX(0, F32- SUM(G32:H32))</f>
+        <v>0</v>
       </c>
       <c r="K32">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f>SUM(G32:H32)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>274</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C33" s="3">
-        <f t="shared" si="0"/>
+        <f>LEN(A33)</f>
         <v>18</v>
       </c>
       <c r="D33" s="3">
-        <v>68</v>
+        <v>275</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">A.18.68    a nye scold hour  </v>
+        <f>CONCATENATE(B33,".",C33,".",D33,"    ",A33)</f>
+        <v xml:space="preserve">A.18.275    on eye scold our  </v>
       </c>
       <c r="F33">
         <v>2</v>
@@ -2690,97 +2669,91 @@
         <v>1</v>
       </c>
       <c r="I33">
-        <f t="shared" si="2"/>
+        <f>MAX(0, F33- SUM(G33:H33))</f>
         <v>1</v>
       </c>
       <c r="K33">
-        <f t="shared" si="3"/>
+        <f>SUM(G33:H33)</f>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>275</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" ref="C34:C65" si="4">LEN(A34)</f>
+        <f>LEN(A34)</f>
         <v>18</v>
       </c>
       <c r="D34" s="3">
-        <v>91</v>
+        <v>276</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" ref="E34:E65" si="5">CONCATENATE(B34,".",C34,".",D34,"    ",A34)</f>
-        <v xml:space="preserve">A.18.91    ah nice cold our  </v>
+        <f>CONCATENATE(B34,".",C34,".",D34,"    ",A34)</f>
+        <v xml:space="preserve">A.18.276    on eye skol dour  </v>
       </c>
       <c r="F34">
-        <v>2</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34">
-        <f t="shared" ref="I34:I65" si="6">MAX(0, F34- SUM(G34:H34))</f>
-        <v>1</v>
+        <f>MAX(0, F34- SUM(G34:H34))</f>
+        <v>0</v>
       </c>
       <c r="K34">
-        <f t="shared" ref="K34:K65" si="7">SUM(G34:H34)</f>
-        <v>1</v>
+        <f>SUM(G34:H34)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>104</v>
-      </c>
-      <c r="B35" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C35" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A35)</f>
+        <v>18</v>
       </c>
       <c r="D35" s="3">
-        <v>105</v>
+        <v>282</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.105    ah nigh scold our  </v>
+        <f>CONCATENATE(B35,".",C35,".",D35,"    ",A35)</f>
+        <v xml:space="preserve">A.18.282    on ice coal dour  </v>
       </c>
       <c r="F35">
-        <v>2</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F35- SUM(G35:H35))</f>
+        <v>0</v>
       </c>
       <c r="K35">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G35:H35)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>283</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C36" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A36)</f>
+        <v>18</v>
       </c>
       <c r="D36" s="3">
-        <v>108</v>
+        <v>284</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.108    ah nye scold hour  </v>
+        <f>CONCATENATE(B36,".",C36,".",D36,"    ",A36)</f>
+        <v xml:space="preserve">A.18.284    on ice cold hour  </v>
       </c>
       <c r="F36">
         <v>2</v>
@@ -2789,97 +2762,91 @@
         <v>1</v>
       </c>
       <c r="I36">
-        <f t="shared" si="6"/>
+        <f>MAX(0, F36- SUM(G36:H36))</f>
         <v>1</v>
       </c>
       <c r="K36">
-        <f t="shared" si="7"/>
+        <f>SUM(G36:H36)</f>
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>110</v>
-      </c>
-      <c r="B37" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C37" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A37)</f>
+        <v>18</v>
       </c>
       <c r="D37" s="3">
-        <v>111</v>
+        <v>286</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.111    ah nye skol dower  </v>
+        <f>CONCATENATE(B37,".",C37,".",D37,"    ",A37)</f>
+        <v xml:space="preserve">A.18.286    on ice cole dour  </v>
       </c>
       <c r="F37">
-        <v>2</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F37- SUM(G37:H37))</f>
+        <v>0</v>
       </c>
       <c r="K37">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G37:H37)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>287</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A38)</f>
+        <v>18</v>
       </c>
       <c r="D38" s="3">
-        <v>116</v>
+        <v>288</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.116    an aye scold hour  </v>
+        <f>CONCATENATE(B38,".",C38,".",D38,"    ",A38)</f>
+        <v xml:space="preserve">A.18.288    on ice kohl dour  </v>
       </c>
       <c r="F38">
-        <v>2</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F38- SUM(G38:H38))</f>
+        <v>0</v>
       </c>
       <c r="K38">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G38:H38)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" t="s">
-        <v>138</v>
-      </c>
-      <c r="B39" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C39" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A39)</f>
+        <v>18</v>
       </c>
       <c r="D39" s="3">
-        <v>139</v>
+        <v>290</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.139    an ice kohl dower  </v>
+        <f>CONCATENATE(B39,".",C39,".",D39,"    ",A39)</f>
+        <v xml:space="preserve">A.18.290    on ice-cold hour  </v>
       </c>
       <c r="F39">
         <v>2</v>
@@ -2888,229 +2855,217 @@
         <v>1</v>
       </c>
       <c r="I39">
-        <f t="shared" si="6"/>
+        <f>MAX(0, F39- SUM(G39:H39))</f>
         <v>1</v>
       </c>
       <c r="K39">
-        <f t="shared" si="7"/>
+        <f>SUM(G39:H39)</f>
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" t="s">
-        <v>159</v>
+        <v>47</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A40)</f>
+        <v>18</v>
       </c>
       <c r="D40" s="3">
-        <v>160</v>
+        <v>48</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.160    eh nice cold hour  </v>
+        <f>CONCATENATE(B40,".",C40,".",D40,"    ",A40)</f>
+        <v xml:space="preserve">A.18.48    a nice coal dour  </v>
       </c>
       <c r="F40">
-        <v>2</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F40- SUM(G40:H40))</f>
+        <v>0</v>
       </c>
       <c r="K40">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G40:H40)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" t="s">
-        <v>174</v>
-      </c>
-      <c r="B41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C41" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A41)</f>
+        <v>18</v>
       </c>
       <c r="D41" s="3">
-        <v>175</v>
+        <v>50</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.175    eh nigh scold our  </v>
+        <f>CONCATENATE(B41,".",C41,".",D41,"    ",A41)</f>
+        <v xml:space="preserve">A.18.50    a nice cold hour  </v>
       </c>
       <c r="F41">
         <v>2</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F41- SUM(G41:H41))</f>
+        <v>2</v>
       </c>
       <c r="K41">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G41:H41)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" t="s">
-        <v>180</v>
+        <v>51</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A42)</f>
+        <v>18</v>
       </c>
       <c r="D42" s="3">
-        <v>181</v>
+        <v>52</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.181    eh nye skol dower  </v>
+        <f>CONCATENATE(B42,".",C42,".",D42,"    ",A42)</f>
+        <v xml:space="preserve">A.18.52    a nice cole dour  </v>
       </c>
       <c r="F42">
-        <v>2</v>
-      </c>
-      <c r="G42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F42- SUM(G42:H42))</f>
+        <v>0</v>
       </c>
       <c r="K42">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G42:H42)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" t="s">
-        <v>268</v>
-      </c>
-      <c r="B43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A43)</f>
+        <v>18</v>
       </c>
       <c r="D43" s="3">
-        <v>269</v>
+        <v>54</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.269    on aye skol dower  </v>
+        <f>CONCATENATE(B43,".",C43,".",D43,"    ",A43)</f>
+        <v xml:space="preserve">A.18.54    a nice kohl dour  </v>
       </c>
       <c r="F43">
-        <v>2</v>
-      </c>
-      <c r="G43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F43- SUM(G43:H43))</f>
+        <v>0</v>
       </c>
       <c r="K43">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G43:H43)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" t="s">
-        <v>273</v>
-      </c>
-      <c r="B44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C44" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A44)</f>
+        <v>18</v>
       </c>
       <c r="D44" s="3">
-        <v>274</v>
+        <v>65</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.274    on eye scold hour  </v>
+        <f>CONCATENATE(B44,".",C44,".",D44,"    ",A44)</f>
+        <v xml:space="preserve">A.18.65    a nigh scold our  </v>
       </c>
       <c r="F44">
         <v>2</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I44">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F44- SUM(G44:H44))</f>
+        <v>0</v>
       </c>
       <c r="K44">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G44:H44)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
-        <v>282</v>
-      </c>
-      <c r="B45" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C45" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A45)</f>
+        <v>18</v>
       </c>
       <c r="D45" s="3">
-        <v>283</v>
+        <v>66</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.283    on ice coal dower  </v>
+        <f>CONCATENATE(B45,".",C45,".",D45,"    ",A45)</f>
+        <v xml:space="preserve">A.18.66    a nigh skol dour  </v>
       </c>
       <c r="F45">
-        <v>2</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F45- SUM(G45:H45))</f>
+        <v>0</v>
       </c>
       <c r="K45">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G45:H45)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" t="s">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C46" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A46)</f>
+        <v>18</v>
       </c>
       <c r="D46" s="3">
-        <v>289</v>
+        <v>68</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.289    on ice kohl dower  </v>
+        <f>CONCATENATE(B46,".",C46,".",D46,"    ",A46)</f>
+        <v xml:space="preserve">A.18.68    a nye scold hour  </v>
       </c>
       <c r="F46">
         <v>2</v>
@@ -3119,97 +3074,97 @@
         <v>1</v>
       </c>
       <c r="I46">
-        <f t="shared" si="6"/>
+        <f>MAX(0, F46- SUM(G46:H46))</f>
         <v>1</v>
       </c>
       <c r="K46">
-        <f t="shared" si="7"/>
+        <f>SUM(G46:H46)</f>
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C47" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A47)</f>
+        <v>18</v>
       </c>
       <c r="D47" s="3">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.49    a nice coal dower  </v>
+        <f>CONCATENATE(B47,".",C47,".",D47,"    ",A47)</f>
+        <v xml:space="preserve">A.18.71    a nye skol dower  </v>
       </c>
       <c r="F47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I47">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f>MAX(0, F47- SUM(G47:H47))</f>
+        <v>0</v>
       </c>
       <c r="K47">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G47:H47)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C48" s="3">
-        <f t="shared" si="4"/>
-        <v>19</v>
+        <f>LEN(A48)</f>
+        <v>18</v>
       </c>
       <c r="D48" s="3">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.64    a nigh scold hour  </v>
+        <f>CONCATENATE(B48,".",C48,".",D48,"    ",A48)</f>
+        <v xml:space="preserve">A.18.91    ah nice cold our  </v>
       </c>
       <c r="F48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G48">
         <v>1</v>
       </c>
       <c r="I48">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f>MAX(0, F48- SUM(G48:H48))</f>
+        <v>1</v>
       </c>
       <c r="K48">
-        <f t="shared" si="7"/>
+        <f>SUM(G48:H48)</f>
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
-        <v>89</v>
-      </c>
-      <c r="B49" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C49" s="3">
-        <f t="shared" si="4"/>
+        <f>LEN(A49)</f>
         <v>19</v>
       </c>
       <c r="D49" s="3">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.19.90    ah nice cold hour  </v>
+        <f>CONCATENATE(B49,".",C49,".",D49,"    ",A49)</f>
+        <v xml:space="preserve">A.19.105    ah nigh scold our  </v>
       </c>
       <c r="F49">
         <v>2</v>
@@ -3218,64 +3173,61 @@
         <v>1</v>
       </c>
       <c r="I49">
-        <f t="shared" si="6"/>
+        <f>MAX(0, F49- SUM(G49:H49))</f>
         <v>1</v>
       </c>
       <c r="K49">
-        <f t="shared" si="7"/>
+        <f>SUM(G49:H49)</f>
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>162</v>
-      </c>
-      <c r="B50" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C50" s="3">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f>LEN(A50)</f>
+        <v>19</v>
       </c>
       <c r="D50" s="3">
-        <v>163</v>
+        <v>106</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.20.163    eh nice cole dower  </v>
+        <f>CONCATENATE(B50,".",C50,".",D50,"    ",A50)</f>
+        <v xml:space="preserve">A.19.106    ah nigh skol dour  </v>
       </c>
       <c r="F50">
-        <v>2</v>
-      </c>
-      <c r="G50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F50- SUM(G50:H50))</f>
+        <v>0</v>
       </c>
       <c r="K50">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G50:H50)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>173</v>
-      </c>
-      <c r="B51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C51" s="3">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f>LEN(A51)</f>
+        <v>19</v>
       </c>
       <c r="D51" s="3">
-        <v>174</v>
+        <v>108</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.20.174    eh nigh scold hour  </v>
+        <f>CONCATENATE(B51,".",C51,".",D51,"    ",A51)</f>
+        <v xml:space="preserve">A.19.108    ah nye scold hour  </v>
       </c>
       <c r="F51">
         <v>2</v>
@@ -3284,31 +3236,31 @@
         <v>1</v>
       </c>
       <c r="I51">
-        <f t="shared" si="6"/>
+        <f>MAX(0, F51- SUM(G51:H51))</f>
         <v>1</v>
       </c>
       <c r="K51">
-        <f t="shared" si="7"/>
+        <f>SUM(G51:H51)</f>
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>176</v>
+        <v>110</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C52" s="3">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f>LEN(A52)</f>
+        <v>19</v>
       </c>
       <c r="D52" s="3">
-        <v>177</v>
+        <v>111</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.20.177    eh nigh skol dower  </v>
+        <f>CONCATENATE(B52,".",C52,".",D52,"    ",A52)</f>
+        <v xml:space="preserve">A.19.111    ah nye skol dower  </v>
       </c>
       <c r="F52">
         <v>2</v>
@@ -3317,31 +3269,31 @@
         <v>1</v>
       </c>
       <c r="I52">
-        <f t="shared" si="6"/>
+        <f>MAX(0, F52- SUM(G52:H52))</f>
         <v>1</v>
       </c>
       <c r="K52">
-        <f t="shared" si="7"/>
+        <f>SUM(G52:H52)</f>
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:11">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C53" s="3">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f>LEN(A53)</f>
+        <v>19</v>
       </c>
       <c r="D53" s="3">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.20.93    ah nice cole dower  </v>
+        <f>CONCATENATE(B53,".",C53,".",D53,"    ",A53)</f>
+        <v xml:space="preserve">A.19.116    an aye scold hour  </v>
       </c>
       <c r="F53">
         <v>2</v>
@@ -3350,196 +3302,196 @@
         <v>1</v>
       </c>
       <c r="I53">
-        <f t="shared" si="6"/>
+        <f>MAX(0, F53- SUM(G53:H53))</f>
         <v>1</v>
       </c>
       <c r="K53">
-        <f t="shared" si="7"/>
+        <f>SUM(G53:H53)</f>
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C54" s="3">
-        <f t="shared" si="4"/>
-        <v>20</v>
+        <f>LEN(A54)</f>
+        <v>19</v>
       </c>
       <c r="D54" s="3">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.20.95    ah nice kohl dower  </v>
+        <f>CONCATENATE(B54,".",C54,".",D54,"    ",A54)</f>
+        <v xml:space="preserve">A.19.119    an aye skol dower  </v>
       </c>
       <c r="F54">
         <v>2</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I54">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F54- SUM(G54:H54))</f>
+        <v>0</v>
       </c>
       <c r="K54">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G54:H54)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" t="s">
-        <v>306</v>
-      </c>
-      <c r="B55" t="s">
-        <v>296</v>
+        <v>123</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="C55" s="3">
-        <f t="shared" si="4"/>
-        <v>15</v>
+        <f>LEN(A55)</f>
+        <v>19</v>
       </c>
       <c r="D55" s="3">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">B.15.10    forth wry two  </v>
+        <f>CONCATENATE(B55,".",C55,".",D55,"    ",A55)</f>
+        <v xml:space="preserve">A.19.124    an eye scold hour  </v>
       </c>
       <c r="F55">
         <v>2</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F55- SUM(G55:H55))</f>
+        <v>2</v>
       </c>
       <c r="K55">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G55:H55)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" t="s">
-        <v>301</v>
-      </c>
-      <c r="B56" t="s">
-        <v>296</v>
+        <v>126</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="C56" s="3">
-        <f t="shared" si="4"/>
-        <v>15</v>
+        <f>LEN(A56)</f>
+        <v>19</v>
       </c>
       <c r="D56" s="3">
-        <v>5</v>
+        <v>127</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">B.15.5    forth rye two  </v>
+        <f>CONCATENATE(B56,".",C56,".",D56,"    ",A56)</f>
+        <v xml:space="preserve">A.19.127    an eye skol dower  </v>
       </c>
       <c r="F56">
         <v>2</v>
       </c>
       <c r="G56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I56">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F56- SUM(G56:H56))</f>
+        <v>0</v>
       </c>
       <c r="K56">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G56:H56)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" t="s">
-        <v>303</v>
-      </c>
-      <c r="B57" t="s">
-        <v>296</v>
+        <v>132</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="C57" s="3">
-        <f t="shared" si="4"/>
-        <v>17</v>
+        <f>LEN(A57)</f>
+        <v>19</v>
       </c>
       <c r="D57" s="3">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">B.17.7    forth write ooh  </v>
+        <f>CONCATENATE(B57,".",C57,".",D57,"    ",A57)</f>
+        <v xml:space="preserve">A.19.133    an ice coal dower  </v>
       </c>
       <c r="F57">
         <v>2</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I57">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F57- SUM(G57:H57))</f>
+        <v>0</v>
       </c>
       <c r="K57">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G57:H57)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" t="s">
-        <v>308</v>
-      </c>
-      <c r="B58" t="s">
-        <v>296</v>
+        <v>136</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="C58" s="3">
-        <f t="shared" si="4"/>
-        <v>18</v>
+        <f>LEN(A58)</f>
+        <v>19</v>
       </c>
       <c r="D58" s="3">
-        <v>12</v>
+        <v>137</v>
       </c>
       <c r="E58" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">B.18.12    fourth right ooh  </v>
+        <f>CONCATENATE(B58,".",C58,".",D58,"    ",A58)</f>
+        <v xml:space="preserve">A.19.137    an ice cole dower  </v>
       </c>
       <c r="F58">
         <v>2</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f>MAX(0, F58- SUM(G58:H58))</f>
+        <v>2</v>
       </c>
       <c r="K58">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f>SUM(G58:H58)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" t="s">
-        <v>313</v>
-      </c>
-      <c r="B59" t="s">
-        <v>296</v>
+        <v>138</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="C59" s="3">
-        <f t="shared" si="4"/>
+        <f>LEN(A59)</f>
         <v>19</v>
       </c>
       <c r="D59" s="3">
-        <v>17</v>
+        <v>139</v>
       </c>
       <c r="E59" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">B.19.17    fourth wright ooh  </v>
+        <f>CONCATENATE(B59,".",C59,".",D59,"    ",A59)</f>
+        <v xml:space="preserve">A.19.139    an ice kohl dower  </v>
       </c>
       <c r="F59">
         <v>2</v>
@@ -3548,400 +3500,415 @@
         <v>1</v>
       </c>
       <c r="I59">
-        <f t="shared" si="6"/>
+        <f>MAX(0, F59- SUM(G59:H59))</f>
         <v>1</v>
       </c>
       <c r="K59">
-        <f t="shared" si="7"/>
+        <f>SUM(G59:H59)</f>
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" t="s">
-        <v>128</v>
-      </c>
-      <c r="B60" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C60" s="3">
-        <f t="shared" si="4"/>
-        <v>16</v>
+        <f>LEN(A60)</f>
+        <v>19</v>
       </c>
       <c r="D60" s="3">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="E60" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.16.129    an i scold our  </v>
+        <f>CONCATENATE(B60,".",C60,".",D60,"    ",A60)</f>
+        <v xml:space="preserve">A.19.158    eh nice coal dour  </v>
       </c>
       <c r="F60">
-        <v>2</v>
-      </c>
-      <c r="G60">
         <v>0</v>
       </c>
       <c r="I60">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f>MAX(0, F60- SUM(G60:H60))</f>
+        <v>0</v>
       </c>
       <c r="K60">
-        <f t="shared" si="7"/>
+        <f>SUM(G60:H60)</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:11">
       <c r="A61" t="s">
-        <v>129</v>
-      </c>
-      <c r="B61" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C61" s="3">
-        <f t="shared" si="4"/>
-        <v>16</v>
+        <f>LEN(A61)</f>
+        <v>19</v>
       </c>
       <c r="D61" s="3">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="E61" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.16.130    an i skol dour  </v>
+        <f>CONCATENATE(B61,".",C61,".",D61,"    ",A61)</f>
+        <v xml:space="preserve">A.19.160    eh nice cold hour  </v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>MAX(0, F61- SUM(G61:H61))</f>
+        <v>1</v>
       </c>
       <c r="K61">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>SUM(G61:H61)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:11">
       <c r="A62" t="s">
-        <v>279</v>
-      </c>
-      <c r="B62" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C62" s="3">
-        <f t="shared" si="4"/>
-        <v>16</v>
+        <f>LEN(A62)</f>
+        <v>19</v>
       </c>
       <c r="D62" s="3">
-        <v>280</v>
+        <v>162</v>
       </c>
       <c r="E62" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.16.280    on i skol dour  </v>
+        <f>CONCATENATE(B62,".",C62,".",D62,"    ",A62)</f>
+        <v xml:space="preserve">A.19.162    eh nice cole dour  </v>
       </c>
       <c r="F62">
         <v>0</v>
       </c>
       <c r="I62">
-        <f t="shared" si="6"/>
+        <f>MAX(0, F62- SUM(G62:H62))</f>
         <v>0</v>
       </c>
       <c r="K62">
-        <f t="shared" si="7"/>
+        <f>SUM(G62:H62)</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:11">
       <c r="A63" t="s">
-        <v>284</v>
+        <v>163</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C63" s="3">
-        <f t="shared" si="4"/>
-        <v>17</v>
+        <f>LEN(A63)</f>
+        <v>19</v>
       </c>
       <c r="D63" s="3">
-        <v>285</v>
+        <v>164</v>
       </c>
       <c r="E63" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.17.285    on ice cold our  </v>
+        <f>CONCATENATE(B63,".",C63,".",D63,"    ",A63)</f>
+        <v xml:space="preserve">A.19.164    eh nice kohl dour  </v>
       </c>
       <c r="F63">
-        <v>2</v>
-      </c>
-      <c r="G63">
         <v>0</v>
       </c>
       <c r="I63">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f>MAX(0, F63- SUM(G63:H63))</f>
+        <v>0</v>
       </c>
       <c r="K63">
-        <f t="shared" si="7"/>
+        <f>SUM(G63:H63)</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" t="s">
-        <v>290</v>
+        <v>174</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C64" s="3">
-        <f t="shared" si="4"/>
-        <v>17</v>
+        <f>LEN(A64)</f>
+        <v>19</v>
       </c>
       <c r="D64" s="3">
-        <v>291</v>
+        <v>175</v>
       </c>
       <c r="E64" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.17.291    on ice-cold our  </v>
+        <f>CONCATENATE(B64,".",C64,".",D64,"    ",A64)</f>
+        <v xml:space="preserve">A.19.175    eh nigh scold our  </v>
       </c>
       <c r="F64">
         <v>2</v>
       </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
       <c r="I64">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f>MAX(0, F64- SUM(G64:H64))</f>
+        <v>1</v>
       </c>
       <c r="K64">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>SUM(G64:H64)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C65" s="3">
-        <f t="shared" si="4"/>
-        <v>17</v>
+        <f>LEN(A65)</f>
+        <v>19</v>
       </c>
       <c r="D65" s="3">
-        <v>70</v>
+        <v>176</v>
       </c>
       <c r="E65" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">A.17.70    a nye skol dour  </v>
+        <f>CONCATENATE(B65,".",C65,".",D65,"    ",A65)</f>
+        <v xml:space="preserve">A.19.176    eh nigh skol dour  </v>
       </c>
       <c r="F65">
         <v>0</v>
       </c>
       <c r="I65">
-        <f t="shared" si="6"/>
+        <f>MAX(0, F65- SUM(G65:H65))</f>
         <v>0</v>
       </c>
       <c r="K65">
-        <f t="shared" si="7"/>
+        <f>SUM(G65:H65)</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:11">
       <c r="A66" t="s">
-        <v>109</v>
+        <v>177</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C66" s="3">
-        <f t="shared" ref="C66:C97" si="8">LEN(A66)</f>
-        <v>18</v>
+        <f>LEN(A66)</f>
+        <v>19</v>
       </c>
       <c r="D66" s="3">
-        <v>110</v>
+        <v>178</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" ref="E66:E97" si="9">CONCATENATE(B66,".",C66,".",D66,"    ",A66)</f>
-        <v xml:space="preserve">A.18.110    ah nye skol dour  </v>
+        <f>CONCATENATE(B66,".",C66,".",D66,"    ",A66)</f>
+        <v xml:space="preserve">A.19.178    eh nye scold hour  </v>
       </c>
       <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66">
         <v>0</v>
       </c>
       <c r="I66">
-        <f t="shared" ref="I66:I97" si="10">MAX(0, F66- SUM(G66:H66))</f>
-        <v>0</v>
+        <f>MAX(0, F66- SUM(G66:H66))</f>
+        <v>2</v>
       </c>
       <c r="K66">
-        <f t="shared" ref="K66:K97" si="11">SUM(G66:H66)</f>
+        <f>SUM(G66:H66)</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:11">
       <c r="A67" t="s">
-        <v>117</v>
-      </c>
-      <c r="B67" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C67" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A67)</f>
+        <v>19</v>
       </c>
       <c r="D67" s="3">
-        <v>118</v>
+        <v>181</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.118    an aye skol dour  </v>
+        <f>CONCATENATE(B67,".",C67,".",D67,"    ",A67)</f>
+        <v xml:space="preserve">A.19.181    eh nye skol dower  </v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
       </c>
       <c r="I67">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F67- SUM(G67:H67))</f>
+        <v>1</v>
       </c>
       <c r="K67">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G67:H67)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" t="s">
-        <v>125</v>
-      </c>
-      <c r="B68" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C68" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A68)</f>
+        <v>19</v>
       </c>
       <c r="D68" s="3">
-        <v>126</v>
+        <v>269</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.126    an eye skol dour  </v>
+        <f>CONCATENATE(B68,".",C68,".",D68,"    ",A68)</f>
+        <v xml:space="preserve">A.19.269    on aye skol dower  </v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
       </c>
       <c r="I68">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F68- SUM(G68:H68))</f>
+        <v>1</v>
       </c>
       <c r="K68">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G68:H68)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:11">
       <c r="A69" t="s">
-        <v>131</v>
-      </c>
-      <c r="B69" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C69" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A69)</f>
+        <v>19</v>
       </c>
       <c r="D69" s="3">
-        <v>132</v>
+        <v>274</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.132    an ice coal dour  </v>
+        <f>CONCATENATE(B69,".",C69,".",D69,"    ",A69)</f>
+        <v xml:space="preserve">A.19.274    on eye scold hour  </v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
       </c>
       <c r="I69">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F69- SUM(G69:H69))</f>
+        <v>1</v>
       </c>
       <c r="K69">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G69:H69)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:11">
       <c r="A70" t="s">
-        <v>135</v>
+        <v>276</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C70" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A70)</f>
+        <v>19</v>
       </c>
       <c r="D70" s="3">
-        <v>136</v>
+        <v>277</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.136    an ice cole dour  </v>
+        <f>CONCATENATE(B70,".",C70,".",D70,"    ",A70)</f>
+        <v xml:space="preserve">A.19.277    on eye skol dower  </v>
       </c>
       <c r="F70">
+        <v>2</v>
+      </c>
+      <c r="G70">
         <v>0</v>
       </c>
       <c r="I70">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F70- SUM(G70:H70))</f>
+        <v>2</v>
       </c>
       <c r="K70">
-        <f t="shared" si="11"/>
+        <f>SUM(G70:H70)</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" t="s">
-        <v>137</v>
-      </c>
-      <c r="B71" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C71" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A71)</f>
+        <v>19</v>
       </c>
       <c r="D71" s="3">
-        <v>138</v>
+        <v>283</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.138    an ice kohl dour  </v>
+        <f>CONCATENATE(B71,".",C71,".",D71,"    ",A71)</f>
+        <v xml:space="preserve">A.19.283    on ice coal dower  </v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
       </c>
       <c r="I71">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F71- SUM(G71:H71))</f>
+        <v>1</v>
       </c>
       <c r="K71">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G71:H71)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" t="s">
-        <v>160</v>
+        <v>286</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C72" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A72)</f>
+        <v>19</v>
       </c>
       <c r="D72" s="3">
-        <v>161</v>
+        <v>287</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.161    eh nice cold our  </v>
+        <f>CONCATENATE(B72,".",C72,".",D72,"    ",A72)</f>
+        <v xml:space="preserve">A.19.287    on ice cole dower  </v>
       </c>
       <c r="F72">
         <v>2</v>
@@ -3950,994 +3917,1039 @@
         <v>0</v>
       </c>
       <c r="I72">
-        <f t="shared" si="10"/>
+        <f>MAX(0, F72- SUM(G72:H72))</f>
         <v>2</v>
       </c>
       <c r="K72">
-        <f t="shared" si="11"/>
+        <f>SUM(G72:H72)</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:11">
       <c r="A73" t="s">
-        <v>179</v>
+        <v>288</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C73" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A73)</f>
+        <v>19</v>
       </c>
       <c r="D73" s="3">
-        <v>180</v>
+        <v>289</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.180    eh nye skol dour  </v>
+        <f>CONCATENATE(B73,".",C73,".",D73,"    ",A73)</f>
+        <v xml:space="preserve">A.19.289    on ice kohl dower  </v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
       </c>
       <c r="I73">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F73- SUM(G73:H73))</f>
+        <v>1</v>
       </c>
       <c r="K73">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G73:H73)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:11">
       <c r="A74" t="s">
-        <v>267</v>
+        <v>48</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C74" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A74)</f>
+        <v>19</v>
       </c>
       <c r="D74" s="3">
-        <v>268</v>
+        <v>49</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.268    on aye skol dour  </v>
+        <f>CONCATENATE(B74,".",C74,".",D74,"    ",A74)</f>
+        <v xml:space="preserve">A.19.49    a nice coal dower  </v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
       </c>
       <c r="I74">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F74- SUM(G74:H74))</f>
+        <v>2</v>
       </c>
       <c r="K74">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G74:H74)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" t="s">
-        <v>275</v>
+        <v>52</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C75" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A75)</f>
+        <v>19</v>
       </c>
       <c r="D75" s="3">
-        <v>276</v>
+        <v>53</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.276    on eye skol dour  </v>
+        <f>CONCATENATE(B75,".",C75,".",D75,"    ",A75)</f>
+        <v xml:space="preserve">A.19.53    a nice cole dower  </v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I75">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F75- SUM(G75:H75))</f>
+        <v>2</v>
       </c>
       <c r="K75">
-        <f t="shared" si="11"/>
+        <f>SUM(G75:H75)</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" t="s">
-        <v>281</v>
-      </c>
-      <c r="B76" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C76" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A76)</f>
+        <v>19</v>
       </c>
       <c r="D76" s="3">
-        <v>282</v>
+        <v>55</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.282    on ice coal dour  </v>
+        <f>CONCATENATE(B76,".",C76,".",D76,"    ",A76)</f>
+        <v xml:space="preserve">A.19.55    a nice kohl dower  </v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I76">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F76- SUM(G76:H76))</f>
+        <v>2</v>
       </c>
       <c r="K76">
-        <f t="shared" si="11"/>
+        <f>SUM(G76:H76)</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:11">
       <c r="A77" t="s">
-        <v>285</v>
-      </c>
-      <c r="B77" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C77" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A77)</f>
+        <v>19</v>
       </c>
       <c r="D77" s="3">
-        <v>286</v>
+        <v>64</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.286    on ice cole dour  </v>
+        <f>CONCATENATE(B77,".",C77,".",D77,"    ",A77)</f>
+        <v xml:space="preserve">A.19.64    a nigh scold hour  </v>
       </c>
       <c r="F77">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
       </c>
       <c r="I77">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F77- SUM(G77:H77))</f>
+        <v>2</v>
       </c>
       <c r="K77">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G77:H77)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:11">
       <c r="A78" t="s">
-        <v>287</v>
+        <v>66</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C78" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A78)</f>
+        <v>19</v>
       </c>
       <c r="D78" s="3">
-        <v>288</v>
+        <v>67</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.288    on ice kohl dour  </v>
+        <f>CONCATENATE(B78,".",C78,".",D78,"    ",A78)</f>
+        <v xml:space="preserve">A.19.67    a nigh skol dower  </v>
       </c>
       <c r="F78">
+        <v>2</v>
+      </c>
+      <c r="G78">
         <v>0</v>
       </c>
       <c r="I78">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F78- SUM(G78:H78))</f>
+        <v>2</v>
       </c>
       <c r="K78">
-        <f t="shared" si="11"/>
+        <f>SUM(G78:H78)</f>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:11">
       <c r="A79" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C79" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A79)</f>
+        <v>19</v>
       </c>
       <c r="D79" s="3">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.48    a nice coal dour  </v>
+        <f>CONCATENATE(B79,".",C79,".",D79,"    ",A79)</f>
+        <v xml:space="preserve">A.19.88    ah nice coal dour  </v>
       </c>
       <c r="F79">
         <v>0</v>
       </c>
       <c r="I79">
-        <f t="shared" si="10"/>
+        <f>MAX(0, F79- SUM(G79:H79))</f>
         <v>0</v>
       </c>
       <c r="K79">
-        <f t="shared" si="11"/>
+        <f>SUM(G79:H79)</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:11">
       <c r="A80" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C80" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A80)</f>
+        <v>19</v>
       </c>
       <c r="D80" s="3">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.50    a nice cold hour  </v>
+        <f>CONCATENATE(B80,".",C80,".",D80,"    ",A80)</f>
+        <v xml:space="preserve">A.19.90    ah nice cold hour  </v>
       </c>
       <c r="F80">
         <v>2</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I80">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f>MAX(0, F80- SUM(G80:H80))</f>
+        <v>1</v>
       </c>
       <c r="K80">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G80:H80)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:11">
       <c r="A81" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C81" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A81)</f>
+        <v>19</v>
       </c>
       <c r="D81" s="3">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.52    a nice cole dour  </v>
+        <f>CONCATENATE(B81,".",C81,".",D81,"    ",A81)</f>
+        <v xml:space="preserve">A.19.92    ah nice cole dour  </v>
       </c>
       <c r="F81">
         <v>0</v>
       </c>
       <c r="I81">
-        <f t="shared" si="10"/>
+        <f>MAX(0, F81- SUM(G81:H81))</f>
         <v>0</v>
       </c>
       <c r="K81">
-        <f t="shared" si="11"/>
+        <f>SUM(G81:H81)</f>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C82" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A82)</f>
+        <v>19</v>
       </c>
       <c r="D82" s="3">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="E82" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.54    a nice kohl dour  </v>
+        <f>CONCATENATE(B82,".",C82,".",D82,"    ",A82)</f>
+        <v xml:space="preserve">A.19.94    ah nice kohl dour  </v>
       </c>
       <c r="F82">
         <v>0</v>
       </c>
       <c r="I82">
-        <f t="shared" si="10"/>
+        <f>MAX(0, F82- SUM(G82:H82))</f>
         <v>0</v>
       </c>
       <c r="K82">
-        <f t="shared" si="11"/>
+        <f>SUM(G82:H82)</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:11">
       <c r="A83" t="s">
-        <v>65</v>
-      </c>
-      <c r="B83" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C83" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
+        <f>LEN(A83)</f>
+        <v>20</v>
       </c>
       <c r="D83" s="3">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="E83" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.18.66    a nigh skol dour  </v>
+        <f>CONCATENATE(B83,".",C83,".",D83,"    ",A83)</f>
+        <v xml:space="preserve">A.20.104    ah nigh scold hour  </v>
       </c>
       <c r="F83">
+        <v>2</v>
+      </c>
+      <c r="G83">
         <v>0</v>
       </c>
       <c r="I83">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F83- SUM(G83:H83))</f>
+        <v>2</v>
       </c>
       <c r="K83">
-        <f t="shared" si="11"/>
+        <f>SUM(G83:H83)</f>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" t="s">
-        <v>105</v>
-      </c>
-      <c r="B84" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C84" s="3">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f>LEN(A84)</f>
+        <v>20</v>
       </c>
       <c r="D84" s="3">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.106    ah nigh skol dour  </v>
+        <f>CONCATENATE(B84,".",C84,".",D84,"    ",A84)</f>
+        <v xml:space="preserve">A.20.107    ah nigh skol dower  </v>
       </c>
       <c r="F84">
+        <v>2</v>
+      </c>
+      <c r="G84">
         <v>0</v>
       </c>
       <c r="I84">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F84- SUM(G84:H84))</f>
+        <v>2</v>
       </c>
       <c r="K84">
-        <f t="shared" si="11"/>
+        <f>SUM(G84:H84)</f>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:11">
       <c r="A85" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C85" s="3">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f>LEN(A85)</f>
+        <v>20</v>
       </c>
       <c r="D85" s="3">
-        <v>124</v>
+        <v>159</v>
       </c>
       <c r="E85" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.124    an eye scold hour  </v>
+        <f>CONCATENATE(B85,".",C85,".",D85,"    ",A85)</f>
+        <v xml:space="preserve">A.20.159    eh nice coal dower  </v>
       </c>
       <c r="F85">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I85">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f>MAX(0, F85- SUM(G85:H85))</f>
+        <v>1</v>
       </c>
       <c r="K85">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G85:H85)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:11">
       <c r="A86" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C86" s="3">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f>LEN(A86)</f>
+        <v>20</v>
       </c>
       <c r="D86" s="3">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="E86" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.137    an ice cole dower  </v>
+        <f>CONCATENATE(B86,".",C86,".",D86,"    ",A86)</f>
+        <v xml:space="preserve">A.20.163    eh nice cole dower  </v>
       </c>
       <c r="F86">
         <v>2</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I86">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f>MAX(0, F86- SUM(G86:H86))</f>
+        <v>1</v>
       </c>
       <c r="K86">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G86:H86)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:11">
       <c r="A87" t="s">
-        <v>157</v>
-      </c>
-      <c r="B87" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C87" s="3">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f>LEN(A87)</f>
+        <v>20</v>
       </c>
       <c r="D87" s="3">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E87" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.158    eh nice coal dour  </v>
+        <f>CONCATENATE(B87,".",C87,".",D87,"    ",A87)</f>
+        <v xml:space="preserve">A.20.165    eh nice kohl dower  </v>
       </c>
       <c r="F87">
+        <v>2</v>
+      </c>
+      <c r="G87">
         <v>0</v>
       </c>
       <c r="I87">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F87- SUM(G87:H87))</f>
+        <v>2</v>
       </c>
       <c r="K87">
-        <f t="shared" si="11"/>
+        <f>SUM(G87:H87)</f>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:11">
       <c r="A88" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>295</v>
       </c>
       <c r="C88" s="3">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f>LEN(A88)</f>
+        <v>20</v>
       </c>
       <c r="D88" s="3">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="E88" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.162    eh nice cole dour  </v>
+        <f>CONCATENATE(B88,".",C88,".",D88,"    ",A88)</f>
+        <v xml:space="preserve">A.20.174    eh nigh scold hour  </v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
       </c>
       <c r="I88">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F88- SUM(G88:H88))</f>
+        <v>1</v>
       </c>
       <c r="K88">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G88:H88)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:11">
       <c r="A89" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C89" s="3">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f>LEN(A89)</f>
+        <v>20</v>
       </c>
       <c r="D89" s="3">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="E89" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.164    eh nice kohl dour  </v>
+        <f>CONCATENATE(B89,".",C89,".",D89,"    ",A89)</f>
+        <v xml:space="preserve">A.20.177    eh nigh skol dower  </v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
       </c>
       <c r="I89">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F89- SUM(G89:H89))</f>
+        <v>1</v>
       </c>
       <c r="K89">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G89:H89)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:11">
       <c r="A90" t="s">
-        <v>175</v>
+        <v>88</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C90" s="3">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f>LEN(A90)</f>
+        <v>20</v>
       </c>
       <c r="D90" s="3">
-        <v>176</v>
+        <v>89</v>
       </c>
       <c r="E90" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.176    eh nigh skol dour  </v>
+        <f>CONCATENATE(B90,".",C90,".",D90,"    ",A90)</f>
+        <v xml:space="preserve">A.20.89    ah nice coal dower  </v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G90">
+        <v>2</v>
       </c>
       <c r="I90">
-        <f t="shared" si="10"/>
+        <f>MAX(0, F90- SUM(G90:H90))</f>
         <v>0</v>
       </c>
       <c r="K90">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G90:H90)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:11">
       <c r="A91" t="s">
-        <v>177</v>
-      </c>
-      <c r="B91" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C91" s="3">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f>LEN(A91)</f>
+        <v>20</v>
       </c>
       <c r="D91" s="3">
-        <v>178</v>
+        <v>93</v>
       </c>
       <c r="E91" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.178    eh nye scold hour  </v>
+        <f>CONCATENATE(B91,".",C91,".",D91,"    ",A91)</f>
+        <v xml:space="preserve">A.20.93    ah nice cole dower  </v>
       </c>
       <c r="F91">
         <v>2</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I91">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f>MAX(0, F91- SUM(G91:H91))</f>
+        <v>1</v>
       </c>
       <c r="K91">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G91:H91)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" t="s">
-        <v>276</v>
+        <v>94</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>295</v>
       </c>
       <c r="C92" s="3">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f>LEN(A92)</f>
+        <v>20</v>
       </c>
       <c r="D92" s="3">
-        <v>277</v>
+        <v>95</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.277    on eye skol dower  </v>
+        <f>CONCATENATE(B92,".",C92,".",D92,"    ",A92)</f>
+        <v xml:space="preserve">A.20.95    ah nice kohl dower  </v>
       </c>
       <c r="F92">
         <v>2</v>
       </c>
       <c r="G92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I92">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f>MAX(0, F92- SUM(G92:H92))</f>
+        <v>1</v>
       </c>
       <c r="K92">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G92:H92)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:11">
       <c r="A93" t="s">
-        <v>286</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>295</v>
+        <v>306</v>
+      </c>
+      <c r="B93" t="s">
+        <v>296</v>
       </c>
       <c r="C93" s="3">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f>LEN(A93)</f>
+        <v>15</v>
       </c>
       <c r="D93" s="3">
-        <v>287</v>
+        <v>10</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.287    on ice cole dower  </v>
+        <f>CONCATENATE(B93,".",C93,".",D93,"    ",A93)</f>
+        <v xml:space="preserve">B.15.10    forth wry two  </v>
       </c>
       <c r="F93">
         <v>2</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I93">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f>MAX(0, F93- SUM(G93:H93))</f>
+        <v>1</v>
       </c>
       <c r="K93">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G93:H93)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" t="s">
-        <v>52</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>295</v>
+        <v>310</v>
+      </c>
+      <c r="B94" t="s">
+        <v>296</v>
       </c>
       <c r="C94" s="3">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f>LEN(A94)</f>
+        <v>15</v>
       </c>
       <c r="D94" s="3">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.53    a nice cole dower  </v>
+        <f>CONCATENATE(B94,".",C94,".",D94,"    ",A94)</f>
+        <v xml:space="preserve">B.15.14    fourth rye to  </v>
       </c>
       <c r="F94">
         <v>2</v>
       </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
       <c r="I94">
-        <f t="shared" si="10"/>
+        <f>MAX(0, F94- SUM(G94:H94))</f>
         <v>2</v>
       </c>
       <c r="K94">
-        <f t="shared" si="11"/>
+        <f>SUM(G94:H94)</f>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:11">
       <c r="A95" t="s">
-        <v>54</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>295</v>
+        <v>315</v>
+      </c>
+      <c r="B95" t="s">
+        <v>296</v>
       </c>
       <c r="C95" s="3">
-        <f t="shared" si="8"/>
+        <f>LEN(A95)</f>
+        <v>15</v>
+      </c>
+      <c r="D95" s="3">
         <v>19</v>
       </c>
-      <c r="D95" s="3">
-        <v>55</v>
-      </c>
       <c r="E95" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.55    a nice kohl dower  </v>
+        <f>CONCATENATE(B95,".",C95,".",D95,"    ",A95)</f>
+        <v xml:space="preserve">B.15.19    fourth wry to  </v>
       </c>
       <c r="F95">
         <v>2</v>
       </c>
+      <c r="G95">
+        <v>2</v>
+      </c>
       <c r="I95">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f>MAX(0, F95- SUM(G95:H95))</f>
+        <v>0</v>
       </c>
       <c r="K95">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>SUM(G95:H95)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:11">
       <c r="A96" t="s">
-        <v>66</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>295</v>
+        <v>301</v>
+      </c>
+      <c r="B96" t="s">
+        <v>296</v>
       </c>
       <c r="C96" s="3">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f>LEN(A96)</f>
+        <v>15</v>
       </c>
       <c r="D96" s="3">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.67    a nigh skol dower  </v>
+        <f>CONCATENATE(B96,".",C96,".",D96,"    ",A96)</f>
+        <v xml:space="preserve">B.15.5    forth rye two  </v>
       </c>
       <c r="F96">
         <v>2</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I96">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f>MAX(0, F96- SUM(G96:H96))</f>
+        <v>1</v>
       </c>
       <c r="K96">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11">
+        <f>SUM(G96:H96)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
       <c r="A97" t="s">
-        <v>87</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>295</v>
+        <v>307</v>
+      </c>
+      <c r="B97" t="s">
+        <v>296</v>
       </c>
       <c r="C97" s="3">
-        <f t="shared" si="8"/>
-        <v>19</v>
+        <f>LEN(A97)</f>
+        <v>16</v>
       </c>
       <c r="D97" s="3">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">A.19.88    ah nice coal dour  </v>
+        <f>CONCATENATE(B97,".",C97,".",D97,"    ",A97)</f>
+        <v xml:space="preserve">B.16.11    forthright ooh  </v>
       </c>
       <c r="F97">
+        <v>2</v>
+      </c>
+      <c r="G97">
         <v>0</v>
       </c>
       <c r="I97">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>MAX(0, F97- SUM(G97:H97))</f>
+        <v>2</v>
       </c>
       <c r="K97">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11">
+        <f>SUM(G97:H97)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="A98" t="s">
-        <v>91</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>295</v>
+        <v>316</v>
+      </c>
+      <c r="B98" t="s">
+        <v>296</v>
       </c>
       <c r="C98" s="3">
-        <f t="shared" ref="C98:C106" si="12">LEN(A98)</f>
-        <v>19</v>
+        <f>LEN(A98)</f>
+        <v>16</v>
       </c>
       <c r="D98" s="3">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" ref="E98:E106" si="13">CONCATENATE(B98,".",C98,".",D98,"    ",A98)</f>
-        <v xml:space="preserve">A.19.92    ah nice cole dour  </v>
+        <f>CONCATENATE(B98,".",C98,".",D98,"    ",A98)</f>
+        <v xml:space="preserve">B.16.20    fourth wry too  </v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G98">
+        <v>2</v>
       </c>
       <c r="I98">
-        <f t="shared" ref="I98:I106" si="14">MAX(0, F98- SUM(G98:H98))</f>
+        <f>MAX(0, F98- SUM(G98:H98))</f>
         <v>0</v>
       </c>
       <c r="K98">
-        <f t="shared" ref="K98:K106" si="15">SUM(G98:H98)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11">
+        <f>SUM(G98:H98)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
       <c r="A99" t="s">
-        <v>93</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>295</v>
+        <v>317</v>
+      </c>
+      <c r="B99" t="s">
+        <v>296</v>
       </c>
       <c r="C99" s="3">
-        <f t="shared" si="12"/>
-        <v>19</v>
+        <f>LEN(A99)</f>
+        <v>16</v>
       </c>
       <c r="D99" s="3">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">A.19.94    ah nice kohl dour  </v>
+        <f>CONCATENATE(B99,".",C99,".",D99,"    ",A99)</f>
+        <v xml:space="preserve">B.16.21    fourth wry two  </v>
       </c>
       <c r="F99">
+        <v>2</v>
+      </c>
+      <c r="G99">
         <v>0</v>
       </c>
       <c r="I99">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f>MAX(0, F99- SUM(G99:H99))</f>
+        <v>2</v>
       </c>
       <c r="K99">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11">
+        <f>SUM(G99:H99)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
       <c r="A100" t="s">
-        <v>103</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
+      </c>
+      <c r="B100" t="s">
+        <v>296</v>
       </c>
       <c r="C100" s="3">
-        <f t="shared" si="12"/>
-        <v>20</v>
+        <f>LEN(A100)</f>
+        <v>17</v>
       </c>
       <c r="D100" s="3">
-        <v>104</v>
+        <v>1</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">A.20.104    ah nigh scold hour  </v>
+        <f>CONCATENATE(B100,".",C100,".",D100,"    ",A100)</f>
+        <v xml:space="preserve">B.17.1    forth right ooh  </v>
       </c>
       <c r="F100">
         <v>2</v>
       </c>
       <c r="G100">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I100">
-        <f t="shared" si="14"/>
-        <v>2</v>
+        <f>MAX(0, F100- SUM(G100:H100))</f>
+        <v>0</v>
       </c>
       <c r="K100">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11">
+        <f>SUM(G100:H100)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="A101" t="s">
-        <v>106</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>295</v>
+        <v>309</v>
+      </c>
+      <c r="B101" t="s">
+        <v>296</v>
       </c>
       <c r="C101" s="3">
-        <f t="shared" si="12"/>
-        <v>20</v>
+        <f>LEN(A101)</f>
+        <v>17</v>
       </c>
       <c r="D101" s="3">
-        <v>107</v>
+        <v>13</v>
       </c>
       <c r="E101" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">A.20.107    ah nigh skol dower  </v>
+        <f>CONCATENATE(B101,".",C101,".",D101,"    ",A101)</f>
+        <v xml:space="preserve">B.17.13    fourth rite ooh  </v>
       </c>
       <c r="F101">
         <v>2</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I101">
-        <f t="shared" si="14"/>
-        <v>2</v>
+        <f>MAX(0, F101- SUM(G101:H101))</f>
+        <v>0</v>
       </c>
       <c r="K101">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11">
+        <f>SUM(G101:H101)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
       <c r="A102" t="s">
-        <v>164</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>295</v>
+        <v>303</v>
+      </c>
+      <c r="B102" t="s">
+        <v>296</v>
       </c>
       <c r="C102" s="3">
-        <f t="shared" si="12"/>
-        <v>20</v>
+        <f>LEN(A102)</f>
+        <v>17</v>
       </c>
       <c r="D102" s="3">
-        <v>165</v>
+        <v>7</v>
       </c>
       <c r="E102" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">A.20.165    eh nice kohl dower  </v>
+        <f>CONCATENATE(B102,".",C102,".",D102,"    ",A102)</f>
+        <v xml:space="preserve">B.17.7    forth write ooh  </v>
       </c>
       <c r="F102">
         <v>2</v>
       </c>
       <c r="G102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I102">
-        <f t="shared" si="14"/>
-        <v>2</v>
+        <f>MAX(0, F102- SUM(G102:H102))</f>
+        <v>1</v>
       </c>
       <c r="K102">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11">
+        <f>SUM(G102:H102)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
       <c r="A103" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B103" t="s">
         <v>296</v>
       </c>
       <c r="C103" s="3">
-        <f t="shared" si="12"/>
-        <v>15</v>
+        <f>LEN(A103)</f>
+        <v>18</v>
       </c>
       <c r="D103" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E103" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">B.15.14    fourth rye to  </v>
+        <f>CONCATENATE(B103,".",C103,".",D103,"    ",A103)</f>
+        <v xml:space="preserve">B.18.12    fourth right ooh  </v>
       </c>
       <c r="F103">
         <v>2</v>
       </c>
       <c r="G103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I103">
-        <f t="shared" si="14"/>
-        <v>2</v>
+        <f>MAX(0, F103- SUM(G103:H103))</f>
+        <v>1</v>
       </c>
       <c r="K103">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11">
+        <f>SUM(G103:H103)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
       <c r="A104" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="B104" t="s">
         <v>296</v>
       </c>
       <c r="C104" s="3">
-        <f t="shared" si="12"/>
-        <v>16</v>
+        <f>LEN(A104)</f>
+        <v>18</v>
       </c>
       <c r="D104" s="3">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E104" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">B.16.11    forthright ooh  </v>
+        <f>CONCATENATE(B104,".",C104,".",D104,"    ",A104)</f>
+        <v xml:space="preserve">B.18.18    fourth write ooh  </v>
       </c>
       <c r="F104">
         <v>2</v>
@@ -4946,84 +4958,118 @@
         <v>0</v>
       </c>
       <c r="I104">
-        <f t="shared" si="14"/>
+        <f>MAX(0, F104- SUM(G104:H104))</f>
         <v>2</v>
       </c>
       <c r="K104">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11">
+        <f>SUM(G104:H104)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
       <c r="A105" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="B105" t="s">
         <v>296</v>
       </c>
       <c r="C105" s="3">
-        <f t="shared" si="12"/>
-        <v>16</v>
+        <f>LEN(A105)</f>
+        <v>18</v>
       </c>
       <c r="D105" s="3">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E105" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">B.16.21    fourth wry two  </v>
+        <f>CONCATENATE(B105,".",C105,".",D105,"    ",A105)</f>
+        <v xml:space="preserve">B.18.6    forth wright ooh  </v>
       </c>
       <c r="F105">
         <v>2</v>
       </c>
       <c r="G105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I105">
-        <f t="shared" si="14"/>
-        <v>2</v>
+        <f>MAX(0, F105- SUM(G105:H105))</f>
+        <v>0</v>
       </c>
       <c r="K105">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11">
+        <f>SUM(G105:H105)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
       <c r="A106" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B106" t="s">
         <v>296</v>
       </c>
       <c r="C106" s="3">
-        <f t="shared" si="12"/>
-        <v>18</v>
+        <f>LEN(A106)</f>
+        <v>19</v>
       </c>
       <c r="D106" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E106" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">B.18.18    fourth write ooh  </v>
+        <f>CONCATENATE(B106,".",C106,".",D106,"    ",A106)</f>
+        <v xml:space="preserve">B.19.17    fourth wright ooh  </v>
       </c>
       <c r="F106">
         <v>2</v>
       </c>
       <c r="G106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I106">
-        <f t="shared" si="14"/>
-        <v>2</v>
+        <f>MAX(0, F106- SUM(G106:H106))</f>
+        <v>1</v>
       </c>
       <c r="K106">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f>SUM(G106:H106)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12">
+      <c r="K107" t="s">
+        <v>325</v>
+      </c>
+      <c r="L107" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12">
+      <c r="J108" t="s">
+        <v>327</v>
+      </c>
+      <c r="K108">
+        <f>COUNTIF(K2:K92,"&gt;0")</f>
+        <v>48</v>
+      </c>
+      <c r="L108">
+        <f>COUNTIF(K93:K106, "&gt;0")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12">
+      <c r="J109" t="s">
+        <v>328</v>
+      </c>
+      <c r="K109">
+        <f>SUM(K2:K92)</f>
+        <v>62</v>
+      </c>
+      <c r="L109">
+        <f>SUM(K93:K106)</f>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K106">
     <sortState ref="A2:K106">
-      <sortCondition descending="1" ref="K1:K106"/>
+      <sortCondition ref="E1:E106"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="I1:I1048576">

</xml_diff>